<commit_message>
check for land assignator for farms
</commit_message>
<xml_diff>
--- a/src/main/data/statistical_data/canton_stats.xlsx
+++ b/src/main/data/statistical_data/canton_stats.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/douglasbouchet/Desktop/swiss_farming_simulator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/douglasbouchet/Desktop/SwissFarmSimulation/src/main/data/statistical_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F93F11A8-2E6E-4346-A014-6E470D866EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2FB28C-30AF-354C-9F50-47AF474BC8CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="17280" windowHeight="18000" xr2:uid="{98662E0A-59F8-1C4D-93E1-B3BF32019C75}"/>
+    <workbookView xWindow="11520" yWindow="500" windowWidth="17280" windowHeight="15640" xr2:uid="{98662E0A-59F8-1C4D-93E1-B3BF32019C75}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -289,26 +289,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -327,6 +309,24 @@
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -645,7 +645,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A78F01E-8977-B047-9AC9-A572E69C8992}">
   <dimension ref="A1:T122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="75" zoomScaleNormal="44" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="75" zoomScaleNormal="44" workbookViewId="0">
       <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
@@ -715,100 +715,100 @@
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="24">
+      <c r="B2" s="14">
         <v>49363</v>
       </c>
-      <c r="C2" s="24">
+      <c r="C2" s="14">
         <v>11174</v>
       </c>
-      <c r="D2" s="34">
+      <c r="D2" s="24">
         <v>24294</v>
       </c>
-      <c r="E2" s="24">
+      <c r="E2" s="14">
         <v>13895</v>
       </c>
-      <c r="F2" s="25">
+      <c r="F2" s="15">
         <v>13.7452170614</v>
       </c>
-      <c r="G2" s="29">
+      <c r="G2" s="19">
         <v>1044033.7061</v>
       </c>
-      <c r="H2" s="24">
+      <c r="H2" s="14">
         <v>15700.208699999999</v>
       </c>
-      <c r="I2" s="24">
+      <c r="I2" s="14">
         <v>1628.3780999999999</v>
       </c>
-      <c r="J2" s="24">
+      <c r="J2" s="14">
         <v>27897.475399999999</v>
       </c>
-      <c r="K2" s="24">
+      <c r="K2" s="14">
         <v>82324.366699999984</v>
       </c>
-      <c r="L2" s="24">
+      <c r="L2" s="14">
         <v>143634.22589999999</v>
       </c>
-      <c r="M2" s="30">
+      <c r="M2" s="20">
         <v>7032</v>
       </c>
-      <c r="N2" s="26">
+      <c r="N2" s="16">
         <v>15.406280216900001</v>
       </c>
-      <c r="O2" s="30">
+      <c r="O2" s="20">
         <v>41284</v>
       </c>
-      <c r="P2" s="16" t="s">
+      <c r="P2" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="31">
+      <c r="B3" s="21">
         <v>3213</v>
       </c>
-      <c r="C3" s="31">
+      <c r="C3" s="21">
         <v>875</v>
       </c>
       <c r="D3">
         <v>1534</v>
       </c>
-      <c r="E3" s="31">
+      <c r="E3" s="21">
         <v>804</v>
       </c>
-      <c r="F3" s="27">
+      <c r="F3" s="17">
         <v>19.063923534899999</v>
       </c>
-      <c r="G3" s="32">
+      <c r="G3" s="22">
         <v>72373.14</v>
       </c>
-      <c r="H3" s="31">
+      <c r="H3" s="21">
         <v>2077.89</v>
       </c>
-      <c r="I3" s="31">
+      <c r="I3" s="21">
         <v>135.5</v>
       </c>
-      <c r="J3" s="31">
+      <c r="J3" s="21">
         <v>2545.09</v>
       </c>
-      <c r="K3" s="31">
+      <c r="K3" s="21">
         <v>7904.65</v>
       </c>
-      <c r="L3" s="31">
+      <c r="L3" s="21">
         <v>13923.09</v>
       </c>
-      <c r="M3" s="33">
+      <c r="M3" s="23">
         <v>412</v>
       </c>
-      <c r="N3" s="28">
+      <c r="N3" s="18">
         <v>13.439219291300001</v>
       </c>
-      <c r="O3" s="33">
+      <c r="O3" s="23">
         <v>1729</v>
       </c>
       <c r="P3" t="s">
@@ -819,46 +819,46 @@
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="31">
+      <c r="B4" s="21">
         <v>10112</v>
       </c>
-      <c r="C4" s="31">
+      <c r="C4" s="21">
         <v>1545</v>
       </c>
       <c r="D4">
         <v>6198</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="21">
         <v>2369</v>
       </c>
-      <c r="F4" s="27">
+      <c r="F4" s="17">
         <v>12.9105186309</v>
       </c>
-      <c r="G4" s="32">
+      <c r="G4" s="22">
         <v>192002.2507</v>
       </c>
-      <c r="H4" s="31">
+      <c r="H4" s="21">
         <v>2360.3465999999999</v>
       </c>
-      <c r="I4" s="31">
+      <c r="I4" s="21">
         <v>437.61090000000002</v>
       </c>
-      <c r="J4" s="31">
+      <c r="J4" s="21">
         <v>5865.5983999999999</v>
       </c>
-      <c r="K4" s="31">
+      <c r="K4" s="21">
         <v>12921.0789</v>
       </c>
-      <c r="L4" s="31">
+      <c r="L4" s="21">
         <v>24772.393800000002</v>
       </c>
-      <c r="M4" s="33">
+      <c r="M4" s="23">
         <v>1313</v>
       </c>
-      <c r="N4" s="28">
+      <c r="N4" s="18">
         <v>12.504970935799999</v>
       </c>
-      <c r="O4" s="33">
+      <c r="O4" s="23">
         <v>5959</v>
       </c>
     </row>
@@ -866,46 +866,46 @@
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="31">
+      <c r="B5" s="21">
         <v>4450</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="21">
         <v>489</v>
       </c>
       <c r="D5">
         <v>2748</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="21">
         <v>1213</v>
       </c>
-      <c r="F5" s="27">
+      <c r="F5" s="17">
         <v>10.4509903566</v>
       </c>
-      <c r="G5" s="32">
+      <c r="G5" s="22">
         <v>75525.154999999999</v>
       </c>
-      <c r="H5" s="31">
+      <c r="H5" s="21">
         <v>912.33709999999996</v>
       </c>
-      <c r="I5" s="31">
+      <c r="I5" s="21">
         <v>68.963300000000004</v>
       </c>
-      <c r="J5" s="31">
+      <c r="J5" s="21">
         <v>2027.4360999999999</v>
       </c>
-      <c r="K5" s="31">
+      <c r="K5" s="21">
         <v>3534.4717000000001</v>
       </c>
-      <c r="L5" s="31">
+      <c r="L5" s="21">
         <v>7913.8876</v>
       </c>
-      <c r="M5" s="33">
+      <c r="M5" s="23">
         <v>419</v>
       </c>
-      <c r="N5" s="28">
+      <c r="N5" s="18">
         <v>10.0729904681</v>
       </c>
-      <c r="O5" s="33">
+      <c r="O5" s="23">
         <v>1493</v>
       </c>
     </row>
@@ -913,46 +913,46 @@
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="31">
+      <c r="B6" s="21">
         <v>540</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="21">
         <v>20</v>
       </c>
       <c r="D6">
         <v>293</v>
       </c>
-      <c r="E6" s="31">
+      <c r="E6" s="21">
         <v>227</v>
       </c>
-      <c r="F6" s="27">
+      <c r="F6" s="17">
         <v>0</v>
       </c>
-      <c r="G6" s="32">
+      <c r="G6" s="22">
         <v>6748.8352999999997</v>
       </c>
-      <c r="H6" s="31">
+      <c r="H6" s="21">
         <v>0</v>
       </c>
-      <c r="I6" s="31">
+      <c r="I6" s="21">
         <v>0</v>
       </c>
-      <c r="J6" s="31">
+      <c r="J6" s="21">
         <v>0</v>
       </c>
-      <c r="K6" s="31">
+      <c r="K6" s="21">
         <v>0</v>
       </c>
-      <c r="L6" s="31">
+      <c r="L6" s="21">
         <v>0</v>
       </c>
-      <c r="M6" s="33">
+      <c r="M6" s="23">
         <v>61</v>
       </c>
-      <c r="N6" s="28">
+      <c r="N6" s="18">
         <v>15.431766269800001</v>
       </c>
-      <c r="O6" s="33">
+      <c r="O6" s="23">
         <v>1076</v>
       </c>
     </row>
@@ -960,46 +960,46 @@
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="31">
+      <c r="B7" s="21">
         <v>1517</v>
       </c>
-      <c r="C7" s="31">
+      <c r="C7" s="21">
         <v>118</v>
       </c>
       <c r="D7">
         <v>902</v>
       </c>
-      <c r="E7" s="31">
+      <c r="E7" s="21">
         <v>497</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F7" s="17">
         <v>0.37330815740000001</v>
       </c>
-      <c r="G7" s="32">
+      <c r="G7" s="22">
         <v>23692.768100000001</v>
       </c>
-      <c r="H7" s="31">
+      <c r="H7" s="21">
         <v>4.4400000000000004</v>
       </c>
-      <c r="I7" s="31">
+      <c r="I7" s="21">
         <v>1.55</v>
       </c>
-      <c r="J7" s="31">
+      <c r="J7" s="21">
         <v>37.42</v>
       </c>
-      <c r="K7" s="31">
+      <c r="K7" s="21">
         <v>30.28</v>
       </c>
-      <c r="L7" s="31">
+      <c r="L7" s="21">
         <v>88.32</v>
       </c>
-      <c r="M7" s="33">
+      <c r="M7" s="23">
         <v>171</v>
       </c>
-      <c r="N7" s="28">
+      <c r="N7" s="18">
         <v>11.9127231734</v>
       </c>
-      <c r="O7" s="33">
+      <c r="O7" s="23">
         <v>906</v>
       </c>
     </row>
@@ -1007,46 +1007,46 @@
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="31">
+      <c r="B8" s="21">
         <v>604</v>
       </c>
-      <c r="C8" s="31">
+      <c r="C8" s="21">
         <v>13</v>
       </c>
       <c r="D8">
         <v>357</v>
       </c>
-      <c r="E8" s="31">
+      <c r="E8" s="21">
         <v>234</v>
       </c>
-      <c r="F8" s="27">
+      <c r="F8" s="17">
         <v>0</v>
       </c>
-      <c r="G8" s="32">
+      <c r="G8" s="22">
         <v>7794.26</v>
       </c>
-      <c r="H8" s="31">
+      <c r="H8" s="21">
         <v>0</v>
       </c>
-      <c r="I8" s="31">
+      <c r="I8" s="21">
         <v>0</v>
       </c>
-      <c r="J8" s="31">
+      <c r="J8" s="21">
         <v>0</v>
       </c>
-      <c r="K8" s="31">
+      <c r="K8" s="21">
         <v>0</v>
       </c>
-      <c r="L8" s="31">
+      <c r="L8" s="21">
         <v>0</v>
       </c>
-      <c r="M8" s="33">
+      <c r="M8" s="23">
         <v>188</v>
       </c>
-      <c r="N8" s="28">
+      <c r="N8" s="18">
         <v>34.797520454500003</v>
       </c>
-      <c r="O8" s="33">
+      <c r="O8" s="23">
         <v>490</v>
       </c>
     </row>
@@ -1054,46 +1054,46 @@
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="31">
+      <c r="B9" s="21">
         <v>417</v>
       </c>
-      <c r="C9" s="31">
+      <c r="C9" s="21">
         <v>12</v>
       </c>
       <c r="D9">
         <v>280</v>
       </c>
-      <c r="E9" s="31">
+      <c r="E9" s="21">
         <v>125</v>
       </c>
-      <c r="F9" s="27">
+      <c r="F9" s="17">
         <v>0</v>
       </c>
-      <c r="G9" s="32">
+      <c r="G9" s="22">
         <v>5916.1232</v>
       </c>
-      <c r="H9" s="31">
+      <c r="H9" s="21">
         <v>0</v>
       </c>
-      <c r="I9" s="31">
+      <c r="I9" s="21">
         <v>0</v>
       </c>
-      <c r="J9" s="31">
+      <c r="J9" s="21">
         <v>0</v>
       </c>
-      <c r="K9" s="31">
+      <c r="K9" s="21">
         <v>0</v>
       </c>
-      <c r="L9" s="31">
+      <c r="L9" s="21">
         <v>0</v>
       </c>
-      <c r="M9" s="33">
+      <c r="M9" s="23">
         <v>79</v>
       </c>
-      <c r="N9" s="28">
+      <c r="N9" s="18">
         <v>19.678747384800001</v>
       </c>
-      <c r="O9" s="33">
+      <c r="O9" s="23">
         <v>275</v>
       </c>
     </row>
@@ -1101,46 +1101,46 @@
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="31">
+      <c r="B10" s="21">
         <v>351</v>
       </c>
-      <c r="C10" s="31">
+      <c r="C10" s="21">
         <v>55</v>
       </c>
       <c r="D10">
         <v>228</v>
       </c>
-      <c r="E10" s="31">
+      <c r="E10" s="21">
         <v>68</v>
       </c>
-      <c r="F10" s="27">
+      <c r="F10" s="17">
         <v>0.22726620559999999</v>
       </c>
-      <c r="G10" s="32">
+      <c r="G10" s="22">
         <v>6919.39</v>
       </c>
-      <c r="H10" s="31">
+      <c r="H10" s="21">
         <v>0</v>
       </c>
-      <c r="I10" s="31">
+      <c r="I10" s="21">
         <v>0</v>
       </c>
-      <c r="J10" s="31">
+      <c r="J10" s="21">
         <v>4.3499999999999996</v>
       </c>
-      <c r="K10" s="31">
+      <c r="K10" s="21">
         <v>9.98</v>
       </c>
-      <c r="L10" s="31">
+      <c r="L10" s="21">
         <v>15.84</v>
       </c>
-      <c r="M10" s="33">
+      <c r="M10" s="23">
         <v>96</v>
       </c>
-      <c r="N10" s="28">
+      <c r="N10" s="18">
         <v>31.019971878700002</v>
       </c>
-      <c r="O10" s="33">
+      <c r="O10" s="23">
         <v>685</v>
       </c>
     </row>
@@ -1148,46 +1148,46 @@
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="31">
+      <c r="B11" s="21">
         <v>547</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="21">
         <v>84</v>
       </c>
       <c r="D11">
         <v>340</v>
       </c>
-      <c r="E11" s="31">
+      <c r="E11" s="21">
         <v>123</v>
       </c>
-      <c r="F11" s="27">
+      <c r="F11" s="17">
         <v>6.6234983975999997</v>
       </c>
-      <c r="G11" s="32">
+      <c r="G11" s="22">
         <v>10609.668799999999</v>
       </c>
-      <c r="H11" s="31">
+      <c r="H11" s="21">
         <v>154.69579999999999</v>
       </c>
-      <c r="I11" s="31">
+      <c r="I11" s="21">
         <v>1.2605999999999999</v>
       </c>
-      <c r="J11" s="31">
+      <c r="J11" s="21">
         <v>120.81189999999999</v>
       </c>
-      <c r="K11" s="31">
+      <c r="K11" s="21">
         <v>319.9178</v>
       </c>
-      <c r="L11" s="31">
+      <c r="L11" s="21">
         <v>705.45259999999996</v>
       </c>
-      <c r="M11" s="33">
+      <c r="M11" s="23">
         <v>87</v>
       </c>
-      <c r="N11" s="28">
+      <c r="N11" s="18">
         <v>16.103122903399999</v>
       </c>
-      <c r="O11" s="33">
+      <c r="O11" s="23">
         <v>238</v>
       </c>
     </row>
@@ -1195,46 +1195,46 @@
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="31">
+      <c r="B12" s="21">
         <v>2690</v>
       </c>
-      <c r="C12" s="31">
+      <c r="C12" s="21">
         <v>1064</v>
       </c>
       <c r="D12">
         <v>1086</v>
       </c>
-      <c r="E12" s="31">
+      <c r="E12" s="21">
         <v>540</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F12" s="17">
         <v>17.126116939500001</v>
       </c>
-      <c r="G12" s="32">
+      <c r="G12" s="22">
         <v>75039.563099999999</v>
       </c>
-      <c r="H12" s="31">
+      <c r="H12" s="21">
         <v>1039.9666999999999</v>
       </c>
-      <c r="I12" s="31">
+      <c r="I12" s="21">
         <v>224.29130000000001</v>
       </c>
-      <c r="J12" s="31">
+      <c r="J12" s="21">
         <v>2414.1142</v>
       </c>
-      <c r="K12" s="31">
+      <c r="K12" s="21">
         <v>7482.8279000000002</v>
       </c>
-      <c r="L12" s="31">
+      <c r="L12" s="21">
         <v>12850.1695</v>
       </c>
-      <c r="M12" s="33">
+      <c r="M12" s="23">
         <v>197</v>
       </c>
-      <c r="N12" s="28">
+      <c r="N12" s="18">
         <v>7.3274824065999997</v>
       </c>
-      <c r="O12" s="33">
+      <c r="O12" s="23">
         <v>1670</v>
       </c>
     </row>
@@ -1242,46 +1242,46 @@
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="31">
+      <c r="B13" s="21">
         <v>1324</v>
       </c>
-      <c r="C13" s="31">
+      <c r="C13" s="21">
         <v>382</v>
       </c>
       <c r="D13">
         <v>663</v>
       </c>
-      <c r="E13" s="31">
+      <c r="E13" s="21">
         <v>279</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F13" s="17">
         <v>17.923468643700001</v>
       </c>
-      <c r="G13" s="32">
+      <c r="G13" s="22">
         <v>31463.404500000001</v>
       </c>
-      <c r="H13" s="31">
+      <c r="H13" s="21">
         <v>523.25070000000005</v>
       </c>
-      <c r="I13" s="31">
+      <c r="I13" s="21">
         <v>81.673299999999998</v>
       </c>
-      <c r="J13" s="31">
+      <c r="J13" s="21">
         <v>1281.5743</v>
       </c>
-      <c r="K13" s="31">
+      <c r="K13" s="21">
         <v>2947.1569</v>
       </c>
-      <c r="L13" s="31">
+      <c r="L13" s="21">
         <v>5642.3522000000003</v>
       </c>
-      <c r="M13" s="33">
+      <c r="M13" s="23">
         <v>168</v>
       </c>
-      <c r="N13" s="28">
+      <c r="N13" s="18">
         <v>15.328849865800001</v>
       </c>
-      <c r="O13" s="33">
+      <c r="O13" s="23">
         <v>790</v>
       </c>
     </row>
@@ -1289,46 +1289,46 @@
       <c r="A14" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="31">
+      <c r="B14" s="21">
         <v>12</v>
       </c>
-      <c r="C14" s="31">
+      <c r="C14" s="21">
         <v>7</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
-      <c r="E14" s="31">
+      <c r="E14" s="21">
         <v>5</v>
       </c>
-      <c r="F14" s="27">
+      <c r="F14" s="17">
         <v>20.905478930899999</v>
       </c>
-      <c r="G14" s="32">
+      <c r="G14" s="22">
         <v>422.75639999999999</v>
       </c>
-      <c r="H14" s="31">
+      <c r="H14" s="21">
         <v>9.3150999999999993</v>
       </c>
-      <c r="I14" s="31">
+      <c r="I14" s="21">
         <v>7.5408999999999997</v>
       </c>
-      <c r="J14" s="31">
+      <c r="J14" s="21">
         <v>11.9269</v>
       </c>
-      <c r="K14" s="31">
+      <c r="K14" s="21">
         <v>44.944200000000002</v>
       </c>
-      <c r="L14" s="31">
+      <c r="L14" s="21">
         <v>88.737799999999993</v>
       </c>
-      <c r="M14" s="33">
+      <c r="M14" s="23">
         <v>4</v>
       </c>
-      <c r="N14" s="28">
+      <c r="N14" s="18">
         <v>40.445801426000003</v>
       </c>
-      <c r="O14" s="33">
+      <c r="O14" s="23">
         <v>37</v>
       </c>
     </row>
@@ -1336,46 +1336,46 @@
       <c r="A15" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="31">
+      <c r="B15" s="21">
         <v>898</v>
       </c>
-      <c r="C15" s="31">
+      <c r="C15" s="21">
         <v>269</v>
       </c>
       <c r="D15">
         <v>407</v>
       </c>
-      <c r="E15" s="31">
+      <c r="E15" s="21">
         <v>222</v>
       </c>
-      <c r="F15" s="27">
+      <c r="F15" s="17">
         <v>15.1629653068</v>
       </c>
-      <c r="G15" s="32">
+      <c r="G15" s="22">
         <v>21436.261200000001</v>
       </c>
-      <c r="H15" s="31">
+      <c r="H15" s="21">
         <v>228.47669999999999</v>
       </c>
-      <c r="I15" s="31">
+      <c r="I15" s="21">
         <v>48.995600000000003</v>
       </c>
-      <c r="J15" s="31">
+      <c r="J15" s="21">
         <v>691.4846</v>
       </c>
-      <c r="K15" s="31">
+      <c r="K15" s="21">
         <v>1674.1712</v>
       </c>
-      <c r="L15" s="31">
+      <c r="L15" s="21">
         <v>3250.3483000000001</v>
       </c>
-      <c r="M15" s="33">
+      <c r="M15" s="23">
         <v>141</v>
       </c>
-      <c r="N15" s="28">
+      <c r="N15" s="18">
         <v>16.252399987699999</v>
       </c>
-      <c r="O15" s="33">
+      <c r="O15" s="23">
         <v>517</v>
       </c>
     </row>
@@ -1383,46 +1383,46 @@
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="31">
+      <c r="B16" s="21">
         <v>523</v>
       </c>
-      <c r="C16" s="31">
+      <c r="C16" s="21">
         <v>216</v>
       </c>
       <c r="D16">
         <v>182</v>
       </c>
-      <c r="E16" s="31">
+      <c r="E16" s="21">
         <v>125</v>
       </c>
-      <c r="F16" s="27">
+      <c r="F16" s="17">
         <v>33.537024289100003</v>
       </c>
-      <c r="G16" s="32">
+      <c r="G16" s="22">
         <v>15955.7601</v>
       </c>
-      <c r="H16" s="31">
+      <c r="H16" s="21">
         <v>387.7955</v>
       </c>
-      <c r="I16" s="31">
+      <c r="I16" s="21">
         <v>67.964299999999994</v>
       </c>
-      <c r="J16" s="31">
+      <c r="J16" s="21">
         <v>956.05640000000005</v>
       </c>
-      <c r="K16" s="31">
+      <c r="K16" s="21">
         <v>3251.3573999999999</v>
       </c>
-      <c r="L16" s="31">
+      <c r="L16" s="21">
         <v>5296.1104999999998</v>
       </c>
-      <c r="M16" s="33">
+      <c r="M16" s="23">
         <v>35</v>
       </c>
-      <c r="N16" s="28">
+      <c r="N16" s="18">
         <v>6.5519213132000003</v>
       </c>
-      <c r="O16" s="33">
+      <c r="O16" s="23">
         <v>298</v>
       </c>
     </row>
@@ -1430,46 +1430,46 @@
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="31">
+      <c r="B17" s="21">
         <v>675</v>
       </c>
-      <c r="C17" s="31">
+      <c r="C17" s="21">
         <v>93</v>
       </c>
       <c r="D17">
         <v>379</v>
       </c>
-      <c r="E17" s="31">
+      <c r="E17" s="21">
         <v>203</v>
       </c>
-      <c r="F17" s="27">
+      <c r="F17" s="17">
         <v>9.8695221E-3</v>
       </c>
-      <c r="G17" s="32">
+      <c r="G17" s="22">
         <v>11873.9375</v>
       </c>
-      <c r="H17" s="31">
+      <c r="H17" s="21">
         <v>0</v>
       </c>
-      <c r="I17" s="31">
+      <c r="I17" s="21">
         <v>0</v>
       </c>
-      <c r="J17" s="31">
+      <c r="J17" s="21">
         <v>0.57999999999999996</v>
       </c>
-      <c r="K17" s="31">
+      <c r="K17" s="21">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="L17" s="31">
+      <c r="L17" s="21">
         <v>1.17</v>
       </c>
-      <c r="M17" s="33">
+      <c r="M17" s="23">
         <v>134</v>
       </c>
-      <c r="N17" s="28">
+      <c r="N17" s="18">
         <v>23.717642655700001</v>
       </c>
-      <c r="O17" s="33">
+      <c r="O17" s="23">
         <v>242</v>
       </c>
     </row>
@@ -1477,46 +1477,46 @@
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="31">
+      <c r="B18" s="21">
         <v>440</v>
       </c>
-      <c r="C18" s="31">
+      <c r="C18" s="21">
         <v>37</v>
       </c>
       <c r="D18">
         <v>271</v>
       </c>
-      <c r="E18" s="31">
+      <c r="E18" s="21">
         <v>132</v>
       </c>
-      <c r="F18" s="27">
+      <c r="F18" s="17">
         <v>0.1503060702</v>
       </c>
-      <c r="G18" s="32">
+      <c r="G18" s="22">
         <v>7111.67</v>
       </c>
-      <c r="H18" s="31">
+      <c r="H18" s="21">
         <v>0.05</v>
       </c>
-      <c r="I18" s="31">
+      <c r="I18" s="21">
         <v>0.05</v>
       </c>
-      <c r="J18" s="31">
+      <c r="J18" s="21">
         <v>0</v>
       </c>
-      <c r="K18" s="31">
+      <c r="K18" s="21">
         <v>0</v>
       </c>
-      <c r="L18" s="31">
+      <c r="L18" s="21">
         <v>10.74</v>
       </c>
-      <c r="M18" s="33">
+      <c r="M18" s="23">
         <v>27</v>
       </c>
-      <c r="N18" s="28">
+      <c r="N18" s="18">
         <v>6.0976121768000002</v>
       </c>
-      <c r="O18" s="33">
+      <c r="O18" s="23">
         <v>172</v>
       </c>
     </row>
@@ -1524,46 +1524,46 @@
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="31">
+      <c r="B19" s="21">
         <v>3860</v>
       </c>
-      <c r="C19" s="31">
+      <c r="C19" s="21">
         <v>602</v>
       </c>
       <c r="D19">
         <v>2212</v>
       </c>
-      <c r="E19" s="31">
+      <c r="E19" s="21">
         <v>1046</v>
       </c>
-      <c r="F19" s="27">
+      <c r="F19" s="17">
         <v>2.0676089047000001</v>
       </c>
-      <c r="G19" s="32">
+      <c r="G19" s="22">
         <v>71295.824900000007</v>
       </c>
-      <c r="H19" s="31">
+      <c r="H19" s="21">
         <v>430.47</v>
       </c>
-      <c r="I19" s="31">
+      <c r="I19" s="21">
         <v>6.44</v>
       </c>
-      <c r="J19" s="31">
+      <c r="J19" s="21">
         <v>295.91000000000003</v>
       </c>
-      <c r="K19" s="31">
+      <c r="K19" s="21">
         <v>631.28530000000001</v>
       </c>
-      <c r="L19" s="31">
+      <c r="L19" s="21">
         <v>1476.3453</v>
       </c>
-      <c r="M19" s="33">
+      <c r="M19" s="23">
         <v>482</v>
       </c>
-      <c r="N19" s="28">
+      <c r="N19" s="18">
         <v>13.3957143016</v>
       </c>
-      <c r="O19" s="33">
+      <c r="O19" s="23">
         <v>2025</v>
       </c>
     </row>
@@ -1571,46 +1571,46 @@
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="31">
+      <c r="B20" s="21">
         <v>2215</v>
       </c>
-      <c r="C20" s="31">
+      <c r="C20" s="21">
         <v>814</v>
       </c>
       <c r="D20">
         <v>935</v>
       </c>
-      <c r="E20" s="31">
+      <c r="E20" s="21">
         <v>466</v>
       </c>
-      <c r="F20" s="27">
+      <c r="F20" s="17">
         <v>1.7840794617</v>
       </c>
-      <c r="G20" s="32">
+      <c r="G20" s="22">
         <v>56251.301599999999</v>
       </c>
-      <c r="H20" s="31">
+      <c r="H20" s="21">
         <v>44.15</v>
       </c>
-      <c r="I20" s="31">
+      <c r="I20" s="21">
         <v>11.62</v>
       </c>
-      <c r="J20" s="31">
+      <c r="J20" s="21">
         <v>281.58</v>
       </c>
-      <c r="K20" s="31">
+      <c r="K20" s="21">
         <v>509.06</v>
       </c>
-      <c r="L20" s="31">
+      <c r="L20" s="21">
         <v>999.65</v>
       </c>
-      <c r="M20" s="33">
+      <c r="M20" s="23">
         <v>1307</v>
       </c>
-      <c r="N20" s="28">
+      <c r="N20" s="18">
         <v>65.169166543100005</v>
       </c>
-      <c r="O20" s="33">
+      <c r="O20" s="23">
         <v>7105</v>
       </c>
     </row>
@@ -1618,46 +1618,46 @@
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="31">
+      <c r="B21" s="21">
         <v>3052</v>
       </c>
-      <c r="C21" s="31">
+      <c r="C21" s="21">
         <v>647</v>
       </c>
       <c r="D21">
         <v>1440</v>
       </c>
-      <c r="E21" s="31">
+      <c r="E21" s="21">
         <v>965</v>
       </c>
-      <c r="F21" s="27">
+      <c r="F21" s="17">
         <v>23.739737123699999</v>
       </c>
-      <c r="G21" s="32">
+      <c r="G21" s="22">
         <v>60132.606</v>
       </c>
-      <c r="H21" s="31">
+      <c r="H21" s="21">
         <v>1897.59</v>
       </c>
-      <c r="I21" s="31">
+      <c r="I21" s="21">
         <v>83.38</v>
       </c>
-      <c r="J21" s="31">
+      <c r="J21" s="21">
         <v>2915.48</v>
       </c>
-      <c r="K21" s="31">
+      <c r="K21" s="21">
         <v>7745.31</v>
       </c>
-      <c r="L21" s="31">
+      <c r="L21" s="21">
         <v>14243.32</v>
       </c>
-      <c r="M21" s="33">
+      <c r="M21" s="23">
         <v>284</v>
       </c>
-      <c r="N21" s="28">
+      <c r="N21" s="18">
         <v>10.314144852</v>
       </c>
-      <c r="O21" s="33">
+      <c r="O21" s="23">
         <v>1403</v>
       </c>
     </row>
@@ -1665,46 +1665,46 @@
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="31">
+      <c r="B22" s="21">
         <v>2491</v>
       </c>
-      <c r="C22" s="31">
+      <c r="C22" s="21">
         <v>529</v>
       </c>
       <c r="D22">
         <v>1242</v>
       </c>
-      <c r="E22" s="31">
+      <c r="E22" s="21">
         <v>720</v>
       </c>
-      <c r="F22" s="27">
+      <c r="F22" s="17">
         <v>16.7271013921</v>
       </c>
-      <c r="G22" s="32">
+      <c r="G22" s="22">
         <v>49433.4692</v>
       </c>
-      <c r="H22" s="31">
+      <c r="H22" s="21">
         <v>1262.5411999999999</v>
       </c>
-      <c r="I22" s="31">
+      <c r="I22" s="21">
         <v>49.249200000000002</v>
       </c>
-      <c r="J22" s="31">
+      <c r="J22" s="21">
         <v>1488.3959</v>
       </c>
-      <c r="K22" s="31">
+      <c r="K22" s="21">
         <v>4973.8627999999999</v>
       </c>
-      <c r="L22" s="31">
+      <c r="L22" s="21">
         <v>8272.5328000000009</v>
       </c>
-      <c r="M22" s="33">
+      <c r="M22" s="23">
         <v>341</v>
       </c>
-      <c r="N22" s="28">
+      <c r="N22" s="18">
         <v>14.3683690487</v>
       </c>
-      <c r="O22" s="33">
+      <c r="O22" s="23">
         <v>991</v>
       </c>
     </row>
@@ -1712,46 +1712,46 @@
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="31">
+      <c r="B23" s="21">
         <v>1055</v>
       </c>
-      <c r="C23" s="31">
+      <c r="C23" s="21">
         <v>130</v>
       </c>
       <c r="D23">
         <v>277</v>
       </c>
-      <c r="E23" s="31">
+      <c r="E23" s="21">
         <v>648</v>
       </c>
-      <c r="F23" s="27">
+      <c r="F23" s="17">
         <v>4.8379205488999997</v>
       </c>
-      <c r="G23" s="32">
+      <c r="G23" s="22">
         <v>13905.962299999999</v>
       </c>
-      <c r="H23" s="31">
+      <c r="H23" s="21">
         <v>305.25479999999999</v>
       </c>
-      <c r="I23" s="31">
+      <c r="I23" s="21">
         <v>0</v>
       </c>
-      <c r="J23" s="31">
+      <c r="J23" s="21">
         <v>19.807300000000001</v>
       </c>
-      <c r="K23" s="31">
+      <c r="K23" s="21">
         <v>214.25069999999999</v>
       </c>
-      <c r="L23" s="31">
+      <c r="L23" s="21">
         <v>663.72879999999998</v>
       </c>
-      <c r="M23" s="33">
+      <c r="M23" s="23">
         <v>146</v>
       </c>
-      <c r="N23" s="28">
+      <c r="N23" s="18">
         <v>20.651717978000001</v>
       </c>
-      <c r="O23" s="33">
+      <c r="O23" s="23">
         <v>2812</v>
       </c>
     </row>
@@ -1759,46 +1759,46 @@
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="31">
+      <c r="B24" s="21">
         <v>3580</v>
       </c>
-      <c r="C24" s="31">
+      <c r="C24" s="21">
         <v>1616</v>
       </c>
       <c r="D24">
         <v>1002</v>
       </c>
-      <c r="E24" s="31">
+      <c r="E24" s="21">
         <v>962</v>
       </c>
-      <c r="F24" s="27">
+      <c r="F24" s="17">
         <v>27.759935522999999</v>
       </c>
-      <c r="G24" s="32">
+      <c r="G24" s="22">
         <v>108345.7632</v>
       </c>
-      <c r="H24" s="31">
+      <c r="H24" s="21">
         <v>3290.8942999999999</v>
       </c>
-      <c r="I24" s="31">
+      <c r="I24" s="21">
         <v>208.88</v>
       </c>
-      <c r="J24" s="31">
+      <c r="J24" s="21">
         <v>4300.8100000000004</v>
       </c>
-      <c r="K24" s="31">
+      <c r="K24" s="21">
         <v>20084.259099999999</v>
       </c>
-      <c r="L24" s="31">
+      <c r="L24" s="21">
         <v>30162.883399999999</v>
       </c>
-      <c r="M24" s="33">
+      <c r="M24" s="23">
         <v>304</v>
       </c>
-      <c r="N24" s="28">
+      <c r="N24" s="18">
         <v>8.6419564509000004</v>
       </c>
-      <c r="O24" s="33">
+      <c r="O24" s="23">
         <v>3212</v>
       </c>
     </row>
@@ -1806,46 +1806,46 @@
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="31">
+      <c r="B25" s="21">
         <v>2634</v>
       </c>
-      <c r="C25" s="31">
+      <c r="C25" s="21">
         <v>323</v>
       </c>
       <c r="D25">
         <v>791</v>
       </c>
-      <c r="E25" s="31">
+      <c r="E25" s="21">
         <v>1520</v>
       </c>
-      <c r="F25" s="27">
+      <c r="F25" s="17">
         <v>2.6045029344000001</v>
       </c>
-      <c r="G25" s="32">
+      <c r="G25" s="22">
         <v>36271.906999999999</v>
       </c>
-      <c r="H25" s="31">
+      <c r="H25" s="21">
         <v>221.52420000000001</v>
       </c>
-      <c r="I25" s="31">
+      <c r="I25" s="21">
         <v>2.0287000000000002</v>
       </c>
-      <c r="J25" s="31">
+      <c r="J25" s="21">
         <v>76.529399999999995</v>
       </c>
-      <c r="K25" s="31">
+      <c r="K25" s="21">
         <v>436.81279999999998</v>
       </c>
-      <c r="L25" s="31">
+      <c r="L25" s="21">
         <v>960.28330000000005</v>
       </c>
-      <c r="M25" s="33">
+      <c r="M25" s="23">
         <v>342</v>
       </c>
-      <c r="N25" s="28">
+      <c r="N25" s="18">
         <v>18.618665221600001</v>
       </c>
-      <c r="O25" s="33">
+      <c r="O25" s="23">
         <v>5224</v>
       </c>
     </row>
@@ -1853,46 +1853,46 @@
       <c r="A26" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="31">
+      <c r="B26" s="21">
         <v>765</v>
       </c>
-      <c r="C26" s="31">
+      <c r="C26" s="21">
         <v>468</v>
       </c>
       <c r="D26">
         <v>167</v>
       </c>
-      <c r="E26" s="31">
+      <c r="E26" s="21">
         <v>130</v>
       </c>
-      <c r="F26" s="27">
+      <c r="F26" s="17">
         <v>7.8786097498999998</v>
       </c>
-      <c r="G26" s="32">
+      <c r="G26" s="22">
         <v>31517.008300000001</v>
       </c>
-      <c r="H26" s="31">
+      <c r="H26" s="21">
         <v>60.27</v>
       </c>
-      <c r="I26" s="31">
+      <c r="I26" s="21">
         <v>65.790000000000006</v>
       </c>
-      <c r="J26" s="31">
+      <c r="J26" s="21">
         <v>596.91</v>
       </c>
-      <c r="K26" s="31">
+      <c r="K26" s="21">
         <v>1332.58</v>
       </c>
-      <c r="L26" s="31">
+      <c r="L26" s="21">
         <v>2483.7600000000002</v>
       </c>
-      <c r="M26" s="33">
+      <c r="M26" s="23">
         <v>87</v>
       </c>
-      <c r="N26" s="28">
+      <c r="N26" s="18">
         <v>8.4942411235000002</v>
       </c>
-      <c r="O26" s="33">
+      <c r="O26" s="23">
         <v>802</v>
       </c>
     </row>
@@ -1900,46 +1900,46 @@
       <c r="A27" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="31">
+      <c r="B27" s="21">
         <v>389</v>
       </c>
-      <c r="C27" s="31">
+      <c r="C27" s="21">
         <v>146</v>
       </c>
       <c r="D27">
         <v>88</v>
       </c>
-      <c r="E27" s="31">
+      <c r="E27" s="21">
         <v>155</v>
       </c>
-      <c r="F27" s="27">
+      <c r="F27" s="17">
         <v>33.6346207729</v>
       </c>
-      <c r="G27" s="32">
+      <c r="G27" s="22">
         <v>11251.09</v>
       </c>
-      <c r="H27" s="31">
+      <c r="H27" s="21">
         <v>309.36</v>
       </c>
-      <c r="I27" s="31">
+      <c r="I27" s="21">
         <v>23.63</v>
       </c>
-      <c r="J27" s="31">
+      <c r="J27" s="21">
         <v>615.39</v>
       </c>
-      <c r="K27" s="31">
+      <c r="K27" s="21">
         <v>2704.56</v>
       </c>
-      <c r="L27" s="31">
+      <c r="L27" s="21">
         <v>3805.31</v>
       </c>
-      <c r="M27" s="33">
+      <c r="M27" s="23">
         <v>41</v>
       </c>
-      <c r="N27" s="28">
+      <c r="N27" s="18">
         <v>11.3578529337</v>
       </c>
-      <c r="O27" s="33">
+      <c r="O27" s="23">
         <v>282</v>
       </c>
     </row>
@@ -1947,46 +1947,46 @@
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="31">
+      <c r="B28" s="21">
         <v>1009</v>
       </c>
-      <c r="C28" s="31">
+      <c r="C28" s="21">
         <v>620</v>
       </c>
       <c r="D28">
         <v>272</v>
       </c>
-      <c r="E28" s="31">
+      <c r="E28" s="21">
         <v>117</v>
       </c>
-      <c r="F28" s="27">
+      <c r="F28" s="17">
         <v>14.853756071099999</v>
       </c>
-      <c r="G28" s="32">
+      <c r="G28" s="22">
         <v>40743.829700000002</v>
       </c>
-      <c r="H28" s="31">
+      <c r="H28" s="21">
         <v>179.59</v>
       </c>
-      <c r="I28" s="31">
+      <c r="I28" s="21">
         <v>101.96</v>
       </c>
-      <c r="J28" s="31">
+      <c r="J28" s="21">
         <v>1350.22</v>
       </c>
-      <c r="K28" s="31">
+      <c r="K28" s="21">
         <v>3571.48</v>
       </c>
-      <c r="L28" s="31">
+      <c r="L28" s="21">
         <v>6007.8</v>
       </c>
-      <c r="M28" s="31">
+      <c r="M28" s="21">
         <v>166</v>
       </c>
-      <c r="N28" s="27">
+      <c r="N28" s="17">
         <v>17.9280731574</v>
       </c>
-      <c r="O28" s="33">
+      <c r="O28" s="23">
         <v>835</v>
       </c>
     </row>
@@ -2005,14 +2005,14 @@
       <c r="B30" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="D30" s="15"/>
-      <c r="E30" s="12" t="s">
+      <c r="D30" s="25"/>
+      <c r="E30" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="F30" s="12"/>
+      <c r="F30" s="34"/>
       <c r="G30" s="2" t="s">
         <v>36</v>
       </c>
@@ -2027,14 +2027,14 @@
       <c r="B31" s="7">
         <v>4956978.3459999999</v>
       </c>
-      <c r="C31" s="14">
+      <c r="C31" s="29">
         <v>4743.6284385153003</v>
       </c>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14">
+      <c r="D31" s="29"/>
+      <c r="E31" s="29">
         <v>786006</v>
       </c>
-      <c r="F31" s="14"/>
+      <c r="F31" s="29"/>
       <c r="G31" s="7">
         <v>1213333.6240000001</v>
       </c>
@@ -2051,14 +2051,14 @@
       <c r="B32" s="4">
         <v>367535.78282135999</v>
       </c>
-      <c r="C32" s="11">
+      <c r="C32" s="26">
         <v>5032.4135682755004</v>
       </c>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11">
+      <c r="D32" s="26"/>
+      <c r="E32" s="26">
         <v>84607.123103959006</v>
       </c>
-      <c r="F32" s="11"/>
+      <c r="F32" s="26"/>
       <c r="G32" s="4">
         <v>79546.385950830998</v>
       </c>
@@ -2073,14 +2073,14 @@
       <c r="B33" s="4">
         <v>790573.43857691996</v>
       </c>
-      <c r="C33" s="11">
+      <c r="C33" s="26">
         <v>4120.1966179320998</v>
       </c>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11">
+      <c r="D33" s="26"/>
+      <c r="E33" s="26">
         <v>160691.23349658001</v>
       </c>
-      <c r="F33" s="11"/>
+      <c r="F33" s="26"/>
       <c r="G33" s="4">
         <v>234277.36790541999</v>
       </c>
@@ -2095,14 +2095,14 @@
       <c r="B34" s="4">
         <v>483491.85653694998</v>
       </c>
-      <c r="C34" s="11">
+      <c r="C34" s="26">
         <v>6384.9391675662</v>
       </c>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11">
+      <c r="D34" s="26"/>
+      <c r="E34" s="26">
         <v>28920.746815546001</v>
       </c>
-      <c r="F34" s="11"/>
+      <c r="F34" s="26"/>
       <c r="G34" s="4">
         <v>106871.96583112</v>
       </c>
@@ -2117,14 +2117,14 @@
       <c r="B35" s="4">
         <v>13127.880841038001</v>
       </c>
-      <c r="C35" s="11">
+      <c r="C35" s="26">
         <v>1943.9784456084001</v>
       </c>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11">
+      <c r="D35" s="26"/>
+      <c r="E35" s="26">
         <v>5.1154354263000004</v>
       </c>
-      <c r="F35" s="11"/>
+      <c r="F35" s="26"/>
       <c r="G35" s="4">
         <v>8425.2740806111997</v>
       </c>
@@ -2139,14 +2139,14 @@
       <c r="B36" s="4">
         <v>58019.01410606</v>
       </c>
-      <c r="C36" s="11">
+      <c r="C36" s="26">
         <v>2452.3331419757001</v>
       </c>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11">
+      <c r="D36" s="26"/>
+      <c r="E36" s="26">
         <v>339.49531817550002</v>
       </c>
-      <c r="F36" s="11"/>
+      <c r="F36" s="26"/>
       <c r="G36" s="4">
         <v>29891.684353421999</v>
       </c>
@@ -2161,14 +2161,14 @@
       <c r="B37" s="4">
         <v>34961.992935404996</v>
       </c>
-      <c r="C37" s="11">
+      <c r="C37" s="26">
         <v>4484.2614646646998</v>
       </c>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11">
+      <c r="D37" s="26"/>
+      <c r="E37" s="26">
         <v>1.4441788682000001</v>
       </c>
-      <c r="F37" s="11"/>
+      <c r="F37" s="26"/>
       <c r="G37" s="4">
         <v>10736.300903747</v>
       </c>
@@ -2183,14 +2183,14 @@
       <c r="B38" s="4">
         <v>17345.379437226002</v>
       </c>
-      <c r="C38" s="11">
+      <c r="C38" s="26">
         <v>2926.6011063687001</v>
       </c>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11">
+      <c r="D38" s="26"/>
+      <c r="E38" s="26">
         <v>18.052235852399999</v>
       </c>
-      <c r="F38" s="11"/>
+      <c r="F38" s="26"/>
       <c r="G38" s="4">
         <v>7745.6980859078003</v>
       </c>
@@ -2205,14 +2205,14 @@
       <c r="B39" s="4">
         <v>22457.544221669999</v>
       </c>
-      <c r="C39" s="11">
+      <c r="C39" s="26">
         <v>3222.1217569615001</v>
       </c>
-      <c r="D39" s="11"/>
-      <c r="E39" s="11">
+      <c r="D39" s="26"/>
+      <c r="E39" s="26">
         <v>64.043111324600005</v>
       </c>
-      <c r="F39" s="11"/>
+      <c r="F39" s="26"/>
       <c r="G39" s="4">
         <v>11</v>
       </c>
@@ -2227,14 +2227,14 @@
       <c r="B40" s="4">
         <v>45780.790559838002</v>
       </c>
-      <c r="C40" s="11">
+      <c r="C40" s="26">
         <v>4298.3429000486003</v>
       </c>
-      <c r="D40" s="11"/>
-      <c r="E40" s="11">
+      <c r="D40" s="26"/>
+      <c r="E40" s="26">
         <v>2535.3539956496002</v>
       </c>
-      <c r="F40" s="11"/>
+      <c r="F40" s="26"/>
       <c r="G40" s="4">
         <v>14660.921634013999</v>
       </c>
@@ -2249,14 +2249,14 @@
       <c r="B41" s="4">
         <v>339106.44353564002</v>
       </c>
-      <c r="C41" s="11">
+      <c r="C41" s="26">
         <v>4519.4547907927999</v>
       </c>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11">
+      <c r="D41" s="26"/>
+      <c r="E41" s="26">
         <v>69599.448877222007</v>
       </c>
-      <c r="F41" s="11"/>
+      <c r="F41" s="26"/>
       <c r="G41" s="4">
         <v>94235.858109088003</v>
       </c>
@@ -2271,14 +2271,14 @@
       <c r="B42" s="4">
         <v>75225.255770980002</v>
       </c>
-      <c r="C42" s="11">
+      <c r="C42" s="26">
         <v>2389.6053954861</v>
       </c>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11">
+      <c r="D42" s="26"/>
+      <c r="E42" s="26">
         <v>26893.706113788001</v>
       </c>
-      <c r="F42" s="11"/>
+      <c r="F42" s="26"/>
       <c r="G42" s="4">
         <v>36449.714810334997</v>
       </c>
@@ -2293,14 +2293,14 @@
       <c r="B43" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="13" t="s">
+      <c r="C43" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13" t="s">
+      <c r="D43" s="27"/>
+      <c r="E43" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="F43" s="13"/>
+      <c r="F43" s="27"/>
       <c r="G43" s="10" t="s">
         <v>31</v>
       </c>
@@ -2315,14 +2315,14 @@
       <c r="B44" s="4">
         <v>71845.928613395998</v>
       </c>
-      <c r="C44" s="11">
+      <c r="C44" s="26">
         <v>3286.5487961628</v>
       </c>
-      <c r="D44" s="11"/>
-      <c r="E44" s="11">
+      <c r="D44" s="26"/>
+      <c r="E44" s="26">
         <v>12636.640261428</v>
       </c>
-      <c r="F44" s="11"/>
+      <c r="F44" s="26"/>
       <c r="G44" s="4">
         <v>26220.550055222</v>
       </c>
@@ -2337,14 +2337,14 @@
       <c r="B45" s="4">
         <v>69521.910218307996</v>
       </c>
-      <c r="C45" s="11">
+      <c r="C45" s="26">
         <v>4402.4056927208003</v>
       </c>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11">
+      <c r="D45" s="26"/>
+      <c r="E45" s="26">
         <v>30931.552146278002</v>
       </c>
-      <c r="F45" s="11"/>
+      <c r="F45" s="26"/>
       <c r="G45" s="4">
         <v>13455.576233948001</v>
       </c>
@@ -2359,14 +2359,14 @@
       <c r="B46" s="4">
         <v>34286.684238684</v>
       </c>
-      <c r="C46" s="11">
+      <c r="C46" s="26">
         <v>2892.2439402670998</v>
       </c>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11">
+      <c r="D46" s="26"/>
+      <c r="E46" s="26">
         <v>7.4430031184000001</v>
       </c>
-      <c r="F46" s="11"/>
+      <c r="F46" s="26"/>
       <c r="G46" s="4">
         <v>15791.405146641</v>
       </c>
@@ -2381,14 +2381,14 @@
       <c r="B47" s="4">
         <v>26062.397327483999</v>
       </c>
-      <c r="C47" s="11">
+      <c r="C47" s="26">
         <v>3647.4371382265999</v>
       </c>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11">
+      <c r="D47" s="26"/>
+      <c r="E47" s="26">
         <v>30.932318284200001</v>
       </c>
-      <c r="F47" s="11"/>
+      <c r="F47" s="26"/>
       <c r="G47" s="4">
         <v>9098.7580289252001</v>
       </c>
@@ -2403,14 +2403,14 @@
       <c r="B48" s="4">
         <v>306636.23944643</v>
       </c>
-      <c r="C48" s="11">
+      <c r="C48" s="26">
         <v>4294.4146918068</v>
       </c>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11">
+      <c r="D48" s="26"/>
+      <c r="E48" s="26">
         <v>10312.198204822</v>
       </c>
-      <c r="F48" s="11"/>
+      <c r="F48" s="26"/>
       <c r="G48" s="4">
         <v>97031.900358654995</v>
       </c>
@@ -2425,14 +2425,14 @@
       <c r="B49" s="4">
         <v>168043.5919497</v>
       </c>
-      <c r="C49" s="11">
+      <c r="C49" s="26">
         <v>2999.0807337578999</v>
       </c>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11">
+      <c r="D49" s="26"/>
+      <c r="E49" s="26">
         <v>4578.4777773425003</v>
       </c>
-      <c r="F49" s="11"/>
+      <c r="F49" s="26"/>
       <c r="G49" s="4">
         <v>60260.898596421997</v>
       </c>
@@ -2447,14 +2447,14 @@
       <c r="B50" s="4">
         <v>315691.20352842001</v>
       </c>
-      <c r="C50" s="11">
+      <c r="C50" s="26">
         <v>5261.7129882831996</v>
       </c>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11">
+      <c r="D50" s="26"/>
+      <c r="E50" s="26">
         <v>67337.303038038997</v>
       </c>
-      <c r="F50" s="11"/>
+      <c r="F50" s="26"/>
       <c r="G50" s="4">
         <v>68500.514683921007</v>
       </c>
@@ -2469,14 +2469,14 @@
       <c r="B51" s="4">
         <v>404753.06168148998</v>
       </c>
-      <c r="C51" s="11">
+      <c r="C51" s="26">
         <v>8184.1208365734001</v>
       </c>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11">
+      <c r="D51" s="26"/>
+      <c r="E51" s="26">
         <v>54666.647685978001</v>
       </c>
-      <c r="F51" s="11"/>
+      <c r="F51" s="26"/>
       <c r="G51" s="4">
         <v>59512.903082156001</v>
       </c>
@@ -2491,14 +2491,14 @@
       <c r="B52" s="4">
         <v>60062.907964227001</v>
       </c>
-      <c r="C52" s="11">
+      <c r="C52" s="26">
         <v>4377.9863378034997</v>
       </c>
-      <c r="D52" s="11"/>
-      <c r="E52" s="11">
+      <c r="D52" s="26"/>
+      <c r="E52" s="26">
         <v>3063.3489903262998</v>
       </c>
-      <c r="F52" s="11"/>
+      <c r="F52" s="26"/>
       <c r="G52" s="4">
         <v>13190.965869324</v>
       </c>
@@ -2513,14 +2513,14 @@
       <c r="B53" s="4">
         <v>585987.36389144999</v>
       </c>
-      <c r="C53" s="11">
+      <c r="C53" s="26">
         <v>5393.0412060375002</v>
       </c>
-      <c r="D53" s="11"/>
-      <c r="E53" s="11">
+      <c r="D53" s="26"/>
+      <c r="E53" s="26">
         <v>172588.86868720001</v>
       </c>
-      <c r="F53" s="11"/>
+      <c r="F53" s="26"/>
       <c r="G53" s="4">
         <v>96180.677173251999</v>
       </c>
@@ -2535,14 +2535,14 @@
       <c r="B54" s="4">
         <v>323692.26819764002</v>
       </c>
-      <c r="C54" s="11">
+      <c r="C54" s="26">
         <v>8779.2620089894008</v>
       </c>
-      <c r="D54" s="11"/>
-      <c r="E54" s="11">
+      <c r="D54" s="26"/>
+      <c r="E54" s="26">
         <v>5990.4473537923004</v>
       </c>
-      <c r="F54" s="11"/>
+      <c r="F54" s="26"/>
       <c r="G54" s="4">
         <v>30877.321384491999</v>
       </c>
@@ -2557,14 +2557,14 @@
       <c r="B55" s="4">
         <v>119009.67327607999</v>
       </c>
-      <c r="C55" s="11">
+      <c r="C55" s="26">
         <v>3775.0408647021</v>
       </c>
-      <c r="D55" s="11"/>
-      <c r="E55" s="11">
+      <c r="D55" s="26"/>
+      <c r="E55" s="26">
         <v>9868.4417303231003</v>
       </c>
-      <c r="F55" s="11"/>
+      <c r="F55" s="26"/>
       <c r="G55" s="4">
         <v>36372.944998935003</v>
       </c>
@@ -2579,14 +2579,14 @@
       <c r="B56" s="4">
         <v>118085.59849824</v>
       </c>
-      <c r="C56" s="11">
+      <c r="C56" s="26">
         <v>10437.398773012999</v>
       </c>
-      <c r="D56" s="11"/>
-      <c r="E56" s="11">
+      <c r="D56" s="26"/>
+      <c r="E56" s="26">
         <v>17055.58471521</v>
       </c>
-      <c r="F56" s="11"/>
+      <c r="F56" s="26"/>
       <c r="G56" s="4">
         <v>5912.5978597676003</v>
       </c>
@@ -2601,14 +2601,14 @@
       <c r="B57" s="4">
         <v>105674.13735413</v>
       </c>
-      <c r="C57" s="11">
+      <c r="C57" s="26">
         <v>2612.7022089568</v>
       </c>
-      <c r="D57" s="11"/>
-      <c r="E57" s="11">
+      <c r="D57" s="26"/>
+      <c r="E57" s="26">
         <v>23262.760456905002</v>
       </c>
-      <c r="F57" s="11"/>
+      <c r="F57" s="26"/>
       <c r="G57" s="4">
         <v>49012.977698084003</v>
       </c>
@@ -2627,7 +2627,7 @@
       <c r="H58" s="2"/>
     </row>
     <row r="65" spans="1:13" ht="31" x14ac:dyDescent="0.35">
-      <c r="A65" s="17"/>
+      <c r="A65" s="11"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
@@ -2647,7 +2647,7 @@
       <c r="C66" s="8"/>
       <c r="D66" s="8"/>
       <c r="E66" s="8"/>
-      <c r="F66" s="18"/>
+      <c r="F66" s="12"/>
       <c r="G66" s="9"/>
       <c r="H66" s="8"/>
       <c r="I66" s="8"/>
@@ -2662,7 +2662,7 @@
       <c r="C67" s="8"/>
       <c r="D67" s="8"/>
       <c r="E67" s="8"/>
-      <c r="F67" s="18"/>
+      <c r="F67" s="12"/>
       <c r="G67" s="9"/>
       <c r="H67" s="8"/>
       <c r="I67" s="8"/>
@@ -2677,7 +2677,7 @@
       <c r="C68" s="8"/>
       <c r="D68" s="8"/>
       <c r="E68" s="8"/>
-      <c r="F68" s="18"/>
+      <c r="F68" s="12"/>
       <c r="G68" s="9"/>
       <c r="H68" s="8"/>
       <c r="I68" s="8"/>
@@ -2692,7 +2692,7 @@
       <c r="C69" s="8"/>
       <c r="D69" s="8"/>
       <c r="E69" s="8"/>
-      <c r="F69" s="18"/>
+      <c r="F69" s="12"/>
       <c r="G69" s="9"/>
       <c r="H69" s="8"/>
       <c r="I69" s="8"/>
@@ -2707,7 +2707,7 @@
       <c r="C70" s="8"/>
       <c r="D70" s="8"/>
       <c r="E70" s="8"/>
-      <c r="F70" s="18"/>
+      <c r="F70" s="12"/>
       <c r="G70" s="9"/>
       <c r="H70" s="8"/>
       <c r="I70" s="8"/>
@@ -2722,7 +2722,7 @@
       <c r="C71" s="8"/>
       <c r="D71" s="8"/>
       <c r="E71" s="8"/>
-      <c r="F71" s="18"/>
+      <c r="F71" s="12"/>
       <c r="G71" s="9"/>
       <c r="H71" s="8"/>
       <c r="I71" s="8"/>
@@ -2737,7 +2737,7 @@
       <c r="C72" s="8"/>
       <c r="D72" s="8"/>
       <c r="E72" s="8"/>
-      <c r="F72" s="18"/>
+      <c r="F72" s="12"/>
       <c r="G72" s="9"/>
       <c r="H72" s="8"/>
       <c r="I72" s="8"/>
@@ -2752,7 +2752,7 @@
       <c r="C73" s="8"/>
       <c r="D73" s="8"/>
       <c r="E73" s="8"/>
-      <c r="F73" s="18"/>
+      <c r="F73" s="12"/>
       <c r="G73" s="9"/>
       <c r="H73" s="8"/>
       <c r="I73" s="8"/>
@@ -2767,7 +2767,7 @@
       <c r="C74" s="8"/>
       <c r="D74" s="8"/>
       <c r="E74" s="8"/>
-      <c r="F74" s="18"/>
+      <c r="F74" s="12"/>
       <c r="G74" s="9"/>
       <c r="H74" s="8"/>
       <c r="I74" s="8"/>
@@ -2782,7 +2782,7 @@
       <c r="C75" s="8"/>
       <c r="D75" s="8"/>
       <c r="E75" s="8"/>
-      <c r="F75" s="18"/>
+      <c r="F75" s="12"/>
       <c r="G75" s="9"/>
       <c r="H75" s="8"/>
       <c r="I75" s="8"/>
@@ -2797,7 +2797,7 @@
       <c r="C76" s="8"/>
       <c r="D76" s="8"/>
       <c r="E76" s="8"/>
-      <c r="F76" s="18"/>
+      <c r="F76" s="12"/>
       <c r="G76" s="9"/>
       <c r="H76" s="8"/>
       <c r="I76" s="8"/>
@@ -2812,7 +2812,7 @@
       <c r="C77" s="8"/>
       <c r="D77" s="8"/>
       <c r="E77" s="8"/>
-      <c r="F77" s="18"/>
+      <c r="F77" s="12"/>
       <c r="G77" s="9"/>
       <c r="H77" s="8"/>
       <c r="I77" s="8"/>
@@ -2827,7 +2827,7 @@
       <c r="C78" s="8"/>
       <c r="D78" s="8"/>
       <c r="E78" s="8"/>
-      <c r="F78" s="18"/>
+      <c r="F78" s="12"/>
       <c r="G78" s="9"/>
       <c r="H78" s="8"/>
       <c r="I78" s="8"/>
@@ -2842,7 +2842,7 @@
       <c r="C79" s="8"/>
       <c r="D79" s="8"/>
       <c r="E79" s="8"/>
-      <c r="F79" s="18"/>
+      <c r="F79" s="12"/>
       <c r="G79" s="9"/>
       <c r="H79" s="8"/>
       <c r="I79" s="8"/>
@@ -2857,7 +2857,7 @@
       <c r="C80" s="8"/>
       <c r="D80" s="8"/>
       <c r="E80" s="8"/>
-      <c r="F80" s="18"/>
+      <c r="F80" s="12"/>
       <c r="G80" s="9"/>
       <c r="H80" s="8"/>
       <c r="I80" s="8"/>
@@ -2872,7 +2872,7 @@
       <c r="C81" s="8"/>
       <c r="D81" s="8"/>
       <c r="E81" s="8"/>
-      <c r="F81" s="18"/>
+      <c r="F81" s="12"/>
       <c r="G81" s="9"/>
       <c r="H81" s="8"/>
       <c r="I81" s="8"/>
@@ -2887,7 +2887,7 @@
       <c r="C82" s="8"/>
       <c r="D82" s="8"/>
       <c r="E82" s="8"/>
-      <c r="F82" s="18"/>
+      <c r="F82" s="12"/>
       <c r="G82" s="9"/>
       <c r="H82" s="8"/>
       <c r="I82" s="8"/>
@@ -2902,7 +2902,7 @@
       <c r="C83" s="8"/>
       <c r="D83" s="8"/>
       <c r="E83" s="8"/>
-      <c r="F83" s="18"/>
+      <c r="F83" s="12"/>
       <c r="G83" s="9"/>
       <c r="H83" s="8"/>
       <c r="I83" s="8"/>
@@ -2917,7 +2917,7 @@
       <c r="C84" s="8"/>
       <c r="D84" s="8"/>
       <c r="E84" s="8"/>
-      <c r="F84" s="18"/>
+      <c r="F84" s="12"/>
       <c r="G84" s="9"/>
       <c r="H84" s="8"/>
       <c r="I84" s="8"/>
@@ -2932,7 +2932,7 @@
       <c r="C85" s="8"/>
       <c r="D85" s="8"/>
       <c r="E85" s="8"/>
-      <c r="F85" s="18"/>
+      <c r="F85" s="12"/>
       <c r="G85" s="9"/>
       <c r="H85" s="8"/>
       <c r="I85" s="8"/>
@@ -2947,7 +2947,7 @@
       <c r="C86" s="8"/>
       <c r="D86" s="8"/>
       <c r="E86" s="8"/>
-      <c r="F86" s="18"/>
+      <c r="F86" s="12"/>
       <c r="G86" s="9"/>
       <c r="H86" s="8"/>
       <c r="I86" s="8"/>
@@ -2962,7 +2962,7 @@
       <c r="C87" s="8"/>
       <c r="D87" s="8"/>
       <c r="E87" s="8"/>
-      <c r="F87" s="18"/>
+      <c r="F87" s="12"/>
       <c r="G87" s="9"/>
       <c r="H87" s="8"/>
       <c r="I87" s="8"/>
@@ -2977,7 +2977,7 @@
       <c r="C88" s="8"/>
       <c r="D88" s="8"/>
       <c r="E88" s="8"/>
-      <c r="F88" s="18"/>
+      <c r="F88" s="12"/>
       <c r="G88" s="9"/>
       <c r="H88" s="8"/>
       <c r="I88" s="8"/>
@@ -2992,7 +2992,7 @@
       <c r="C89" s="8"/>
       <c r="D89" s="8"/>
       <c r="E89" s="8"/>
-      <c r="F89" s="18"/>
+      <c r="F89" s="12"/>
       <c r="G89" s="9"/>
       <c r="H89" s="8"/>
       <c r="I89" s="8"/>
@@ -3007,7 +3007,7 @@
       <c r="C90" s="8"/>
       <c r="D90" s="8"/>
       <c r="E90" s="8"/>
-      <c r="F90" s="18"/>
+      <c r="F90" s="12"/>
       <c r="G90" s="9"/>
       <c r="H90" s="8"/>
       <c r="I90" s="8"/>
@@ -3022,7 +3022,7 @@
       <c r="C91" s="8"/>
       <c r="D91" s="8"/>
       <c r="E91" s="8"/>
-      <c r="F91" s="18"/>
+      <c r="F91" s="12"/>
       <c r="G91" s="9"/>
       <c r="H91" s="8"/>
       <c r="I91" s="8"/>
@@ -3037,7 +3037,7 @@
       <c r="C92" s="8"/>
       <c r="D92" s="8"/>
       <c r="E92" s="8"/>
-      <c r="F92" s="18"/>
+      <c r="F92" s="12"/>
       <c r="G92" s="9"/>
       <c r="H92" s="8"/>
       <c r="I92" s="8"/>
@@ -3062,12 +3062,12 @@
       <c r="M93" s="1"/>
     </row>
     <row r="94" spans="1:13" ht="31" x14ac:dyDescent="0.35">
-      <c r="A94" s="17"/>
+      <c r="A94" s="11"/>
       <c r="B94" s="3"/>
-      <c r="C94" s="19"/>
-      <c r="D94" s="19"/>
-      <c r="E94" s="20"/>
-      <c r="F94" s="20"/>
+      <c r="C94" s="30"/>
+      <c r="D94" s="30"/>
+      <c r="E94" s="31"/>
+      <c r="F94" s="31"/>
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
       <c r="I94" s="1"/>
@@ -3079,10 +3079,10 @@
     <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95" s="3"/>
       <c r="B95" s="8"/>
-      <c r="C95" s="21"/>
-      <c r="D95" s="21"/>
-      <c r="E95" s="21"/>
-      <c r="F95" s="21"/>
+      <c r="C95" s="28"/>
+      <c r="D95" s="28"/>
+      <c r="E95" s="28"/>
+      <c r="F95" s="28"/>
       <c r="G95" s="8"/>
       <c r="H95" s="8"/>
       <c r="I95" s="1"/>
@@ -3094,10 +3094,10 @@
     <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96" s="3"/>
       <c r="B96" s="8"/>
-      <c r="C96" s="21"/>
-      <c r="D96" s="21"/>
-      <c r="E96" s="21"/>
-      <c r="F96" s="21"/>
+      <c r="C96" s="28"/>
+      <c r="D96" s="28"/>
+      <c r="E96" s="28"/>
+      <c r="F96" s="28"/>
       <c r="G96" s="8"/>
       <c r="H96" s="8"/>
       <c r="I96" s="1"/>
@@ -3109,10 +3109,10 @@
     <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97" s="3"/>
       <c r="B97" s="8"/>
-      <c r="C97" s="21"/>
-      <c r="D97" s="21"/>
-      <c r="E97" s="21"/>
-      <c r="F97" s="21"/>
+      <c r="C97" s="28"/>
+      <c r="D97" s="28"/>
+      <c r="E97" s="28"/>
+      <c r="F97" s="28"/>
       <c r="G97" s="8"/>
       <c r="H97" s="8"/>
       <c r="I97" s="1"/>
@@ -3124,10 +3124,10 @@
     <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98" s="3"/>
       <c r="B98" s="8"/>
-      <c r="C98" s="21"/>
-      <c r="D98" s="21"/>
-      <c r="E98" s="21"/>
-      <c r="F98" s="21"/>
+      <c r="C98" s="28"/>
+      <c r="D98" s="28"/>
+      <c r="E98" s="28"/>
+      <c r="F98" s="28"/>
       <c r="G98" s="8"/>
       <c r="H98" s="8"/>
       <c r="I98" s="1"/>
@@ -3139,10 +3139,10 @@
     <row r="99" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A99" s="3"/>
       <c r="B99" s="8"/>
-      <c r="C99" s="21"/>
-      <c r="D99" s="21"/>
-      <c r="E99" s="21"/>
-      <c r="F99" s="21"/>
+      <c r="C99" s="28"/>
+      <c r="D99" s="28"/>
+      <c r="E99" s="28"/>
+      <c r="F99" s="28"/>
       <c r="G99" s="8"/>
       <c r="H99" s="8"/>
       <c r="I99" s="1"/>
@@ -3154,10 +3154,10 @@
     <row r="100" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A100" s="3"/>
       <c r="B100" s="8"/>
-      <c r="C100" s="21"/>
-      <c r="D100" s="21"/>
-      <c r="E100" s="21"/>
-      <c r="F100" s="21"/>
+      <c r="C100" s="28"/>
+      <c r="D100" s="28"/>
+      <c r="E100" s="28"/>
+      <c r="F100" s="28"/>
       <c r="G100" s="8"/>
       <c r="H100" s="8"/>
       <c r="I100" s="1"/>
@@ -3169,10 +3169,10 @@
     <row r="101" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A101" s="3"/>
       <c r="B101" s="8"/>
-      <c r="C101" s="21"/>
-      <c r="D101" s="21"/>
-      <c r="E101" s="21"/>
-      <c r="F101" s="21"/>
+      <c r="C101" s="28"/>
+      <c r="D101" s="28"/>
+      <c r="E101" s="28"/>
+      <c r="F101" s="28"/>
       <c r="G101" s="8"/>
       <c r="H101" s="8"/>
       <c r="I101" s="1"/>
@@ -3184,10 +3184,10 @@
     <row r="102" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A102" s="3"/>
       <c r="B102" s="8"/>
-      <c r="C102" s="21"/>
-      <c r="D102" s="21"/>
-      <c r="E102" s="21"/>
-      <c r="F102" s="21"/>
+      <c r="C102" s="28"/>
+      <c r="D102" s="28"/>
+      <c r="E102" s="28"/>
+      <c r="F102" s="28"/>
       <c r="G102" s="8"/>
       <c r="H102" s="8"/>
       <c r="I102" s="1"/>
@@ -3199,10 +3199,10 @@
     <row r="103" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A103" s="3"/>
       <c r="B103" s="8"/>
-      <c r="C103" s="21"/>
-      <c r="D103" s="21"/>
-      <c r="E103" s="21"/>
-      <c r="F103" s="21"/>
+      <c r="C103" s="28"/>
+      <c r="D103" s="28"/>
+      <c r="E103" s="28"/>
+      <c r="F103" s="28"/>
       <c r="G103" s="8"/>
       <c r="H103" s="8"/>
       <c r="I103" s="1"/>
@@ -3214,10 +3214,10 @@
     <row r="104" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A104" s="3"/>
       <c r="B104" s="8"/>
-      <c r="C104" s="21"/>
-      <c r="D104" s="21"/>
-      <c r="E104" s="21"/>
-      <c r="F104" s="21"/>
+      <c r="C104" s="28"/>
+      <c r="D104" s="28"/>
+      <c r="E104" s="28"/>
+      <c r="F104" s="28"/>
       <c r="G104" s="8"/>
       <c r="H104" s="8"/>
       <c r="I104" s="1"/>
@@ -3229,10 +3229,10 @@
     <row r="105" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A105" s="3"/>
       <c r="B105" s="8"/>
-      <c r="C105" s="21"/>
-      <c r="D105" s="21"/>
-      <c r="E105" s="21"/>
-      <c r="F105" s="21"/>
+      <c r="C105" s="28"/>
+      <c r="D105" s="28"/>
+      <c r="E105" s="28"/>
+      <c r="F105" s="28"/>
       <c r="G105" s="8"/>
       <c r="H105" s="8"/>
       <c r="I105" s="1"/>
@@ -3244,10 +3244,10 @@
     <row r="106" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A106" s="3"/>
       <c r="B106" s="8"/>
-      <c r="C106" s="21"/>
-      <c r="D106" s="21"/>
-      <c r="E106" s="21"/>
-      <c r="F106" s="21"/>
+      <c r="C106" s="28"/>
+      <c r="D106" s="28"/>
+      <c r="E106" s="28"/>
+      <c r="F106" s="28"/>
       <c r="G106" s="8"/>
       <c r="H106" s="8"/>
       <c r="I106" s="1"/>
@@ -3258,13 +3258,13 @@
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A107" s="3"/>
-      <c r="B107" s="22"/>
-      <c r="C107" s="23"/>
-      <c r="D107" s="23"/>
-      <c r="E107" s="23"/>
-      <c r="F107" s="23"/>
-      <c r="G107" s="22"/>
-      <c r="H107" s="22"/>
+      <c r="B107" s="13"/>
+      <c r="C107" s="33"/>
+      <c r="D107" s="33"/>
+      <c r="E107" s="33"/>
+      <c r="F107" s="33"/>
+      <c r="G107" s="13"/>
+      <c r="H107" s="13"/>
       <c r="I107" s="1"/>
       <c r="J107" s="1"/>
       <c r="K107" s="1"/>
@@ -3274,10 +3274,10 @@
     <row r="108" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A108" s="3"/>
       <c r="B108" s="8"/>
-      <c r="C108" s="21"/>
-      <c r="D108" s="21"/>
-      <c r="E108" s="21"/>
-      <c r="F108" s="21"/>
+      <c r="C108" s="28"/>
+      <c r="D108" s="28"/>
+      <c r="E108" s="28"/>
+      <c r="F108" s="28"/>
       <c r="G108" s="8"/>
       <c r="H108" s="8"/>
       <c r="I108" s="1"/>
@@ -3289,10 +3289,10 @@
     <row r="109" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A109" s="3"/>
       <c r="B109" s="8"/>
-      <c r="C109" s="21"/>
-      <c r="D109" s="21"/>
-      <c r="E109" s="21"/>
-      <c r="F109" s="21"/>
+      <c r="C109" s="28"/>
+      <c r="D109" s="28"/>
+      <c r="E109" s="28"/>
+      <c r="F109" s="28"/>
       <c r="G109" s="8"/>
       <c r="H109" s="8"/>
       <c r="I109" s="1"/>
@@ -3304,10 +3304,10 @@
     <row r="110" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A110" s="3"/>
       <c r="B110" s="8"/>
-      <c r="C110" s="21"/>
-      <c r="D110" s="21"/>
-      <c r="E110" s="21"/>
-      <c r="F110" s="21"/>
+      <c r="C110" s="28"/>
+      <c r="D110" s="28"/>
+      <c r="E110" s="28"/>
+      <c r="F110" s="28"/>
       <c r="G110" s="8"/>
       <c r="H110" s="8"/>
       <c r="I110" s="1"/>
@@ -3319,10 +3319,10 @@
     <row r="111" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A111" s="3"/>
       <c r="B111" s="8"/>
-      <c r="C111" s="21"/>
-      <c r="D111" s="21"/>
-      <c r="E111" s="21"/>
-      <c r="F111" s="21"/>
+      <c r="C111" s="28"/>
+      <c r="D111" s="28"/>
+      <c r="E111" s="28"/>
+      <c r="F111" s="28"/>
       <c r="G111" s="8"/>
       <c r="H111" s="8"/>
       <c r="I111" s="1"/>
@@ -3334,10 +3334,10 @@
     <row r="112" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A112" s="3"/>
       <c r="B112" s="8"/>
-      <c r="C112" s="21"/>
-      <c r="D112" s="21"/>
-      <c r="E112" s="21"/>
-      <c r="F112" s="21"/>
+      <c r="C112" s="28"/>
+      <c r="D112" s="28"/>
+      <c r="E112" s="28"/>
+      <c r="F112" s="28"/>
       <c r="G112" s="8"/>
       <c r="H112" s="8"/>
       <c r="I112" s="1"/>
@@ -3349,10 +3349,10 @@
     <row r="113" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A113" s="3"/>
       <c r="B113" s="8"/>
-      <c r="C113" s="21"/>
-      <c r="D113" s="21"/>
-      <c r="E113" s="21"/>
-      <c r="F113" s="21"/>
+      <c r="C113" s="28"/>
+      <c r="D113" s="28"/>
+      <c r="E113" s="28"/>
+      <c r="F113" s="28"/>
       <c r="G113" s="8"/>
       <c r="H113" s="8"/>
       <c r="I113" s="1"/>
@@ -3364,10 +3364,10 @@
     <row r="114" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A114" s="3"/>
       <c r="B114" s="8"/>
-      <c r="C114" s="21"/>
-      <c r="D114" s="21"/>
-      <c r="E114" s="21"/>
-      <c r="F114" s="21"/>
+      <c r="C114" s="28"/>
+      <c r="D114" s="28"/>
+      <c r="E114" s="28"/>
+      <c r="F114" s="28"/>
       <c r="G114" s="8"/>
       <c r="H114" s="8"/>
       <c r="I114" s="1"/>
@@ -3379,10 +3379,10 @@
     <row r="115" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A115" s="3"/>
       <c r="B115" s="8"/>
-      <c r="C115" s="21"/>
-      <c r="D115" s="21"/>
-      <c r="E115" s="21"/>
-      <c r="F115" s="21"/>
+      <c r="C115" s="28"/>
+      <c r="D115" s="28"/>
+      <c r="E115" s="28"/>
+      <c r="F115" s="28"/>
       <c r="G115" s="8"/>
       <c r="H115" s="8"/>
       <c r="I115" s="1"/>
@@ -3394,10 +3394,10 @@
     <row r="116" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A116" s="3"/>
       <c r="B116" s="8"/>
-      <c r="C116" s="21"/>
-      <c r="D116" s="21"/>
-      <c r="E116" s="21"/>
-      <c r="F116" s="21"/>
+      <c r="C116" s="28"/>
+      <c r="D116" s="28"/>
+      <c r="E116" s="28"/>
+      <c r="F116" s="28"/>
       <c r="G116" s="8"/>
       <c r="H116" s="8"/>
       <c r="I116" s="1"/>
@@ -3409,10 +3409,10 @@
     <row r="117" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A117" s="3"/>
       <c r="B117" s="8"/>
-      <c r="C117" s="21"/>
-      <c r="D117" s="21"/>
-      <c r="E117" s="21"/>
-      <c r="F117" s="21"/>
+      <c r="C117" s="28"/>
+      <c r="D117" s="28"/>
+      <c r="E117" s="28"/>
+      <c r="F117" s="28"/>
       <c r="G117" s="8"/>
       <c r="H117" s="8"/>
       <c r="I117" s="1"/>
@@ -3424,10 +3424,10 @@
     <row r="118" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A118" s="3"/>
       <c r="B118" s="8"/>
-      <c r="C118" s="21"/>
-      <c r="D118" s="21"/>
-      <c r="E118" s="21"/>
-      <c r="F118" s="21"/>
+      <c r="C118" s="28"/>
+      <c r="D118" s="28"/>
+      <c r="E118" s="28"/>
+      <c r="F118" s="28"/>
       <c r="G118" s="8"/>
       <c r="H118" s="8"/>
       <c r="I118" s="1"/>
@@ -3439,10 +3439,10 @@
     <row r="119" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A119" s="3"/>
       <c r="B119" s="8"/>
-      <c r="C119" s="21"/>
-      <c r="D119" s="21"/>
-      <c r="E119" s="21"/>
-      <c r="F119" s="21"/>
+      <c r="C119" s="28"/>
+      <c r="D119" s="28"/>
+      <c r="E119" s="28"/>
+      <c r="F119" s="28"/>
       <c r="G119" s="8"/>
       <c r="H119" s="8"/>
       <c r="I119" s="1"/>
@@ -3454,10 +3454,10 @@
     <row r="120" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A120" s="3"/>
       <c r="B120" s="8"/>
-      <c r="C120" s="21"/>
-      <c r="D120" s="21"/>
-      <c r="E120" s="21"/>
-      <c r="F120" s="21"/>
+      <c r="C120" s="28"/>
+      <c r="D120" s="28"/>
+      <c r="E120" s="28"/>
+      <c r="F120" s="28"/>
       <c r="G120" s="8"/>
       <c r="H120" s="8"/>
       <c r="I120" s="1"/>
@@ -3469,10 +3469,10 @@
     <row r="121" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A121" s="3"/>
       <c r="B121" s="8"/>
-      <c r="C121" s="21"/>
-      <c r="D121" s="21"/>
-      <c r="E121" s="21"/>
-      <c r="F121" s="21"/>
+      <c r="C121" s="28"/>
+      <c r="D121" s="28"/>
+      <c r="E121" s="28"/>
+      <c r="F121" s="28"/>
       <c r="G121" s="8"/>
       <c r="H121" s="8"/>
       <c r="I121" s="1"/>
@@ -3498,6 +3498,95 @@
     </row>
   </sheetData>
   <mergeCells count="113">
+    <mergeCell ref="C112:D112"/>
+    <mergeCell ref="E112:F112"/>
+    <mergeCell ref="C113:D113"/>
+    <mergeCell ref="E113:F113"/>
+    <mergeCell ref="C114:D114"/>
+    <mergeCell ref="E114:F114"/>
+    <mergeCell ref="C109:D109"/>
+    <mergeCell ref="C121:D121"/>
+    <mergeCell ref="E121:F121"/>
+    <mergeCell ref="C118:D118"/>
+    <mergeCell ref="E118:F118"/>
+    <mergeCell ref="C119:D119"/>
+    <mergeCell ref="E119:F119"/>
+    <mergeCell ref="C120:D120"/>
+    <mergeCell ref="E120:F120"/>
+    <mergeCell ref="C115:D115"/>
+    <mergeCell ref="E115:F115"/>
+    <mergeCell ref="C116:D116"/>
+    <mergeCell ref="E116:F116"/>
+    <mergeCell ref="C117:D117"/>
+    <mergeCell ref="E117:F117"/>
+    <mergeCell ref="E109:F109"/>
+    <mergeCell ref="C110:D110"/>
+    <mergeCell ref="E110:F110"/>
+    <mergeCell ref="C111:D111"/>
+    <mergeCell ref="E111:F111"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="E106:F106"/>
+    <mergeCell ref="C107:D107"/>
+    <mergeCell ref="E107:F107"/>
+    <mergeCell ref="C108:D108"/>
+    <mergeCell ref="E108:F108"/>
+    <mergeCell ref="P2:T2"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="C103:D103"/>
+    <mergeCell ref="E103:F103"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="E104:F104"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="E105:F105"/>
+    <mergeCell ref="C100:D100"/>
+    <mergeCell ref="E100:F100"/>
+    <mergeCell ref="C101:D101"/>
+    <mergeCell ref="E101:F101"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="E102:F102"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="E97:F97"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="E98:F98"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="E99:F99"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="E94:F94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="E95:F95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="E96:F96"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E47:F47"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="C57:D57"/>
     <mergeCell ref="E32:F32"/>
@@ -3522,95 +3611,6 @@
     <mergeCell ref="C39:D39"/>
     <mergeCell ref="C40:D40"/>
     <mergeCell ref="C41:D41"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="E97:F97"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="E98:F98"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="E99:F99"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="E94:F94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="E95:F95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="E96:F96"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="P2:T2"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="C103:D103"/>
-    <mergeCell ref="E103:F103"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="E104:F104"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="E105:F105"/>
-    <mergeCell ref="C100:D100"/>
-    <mergeCell ref="E100:F100"/>
-    <mergeCell ref="C101:D101"/>
-    <mergeCell ref="E101:F101"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="E102:F102"/>
-    <mergeCell ref="E109:F109"/>
-    <mergeCell ref="C110:D110"/>
-    <mergeCell ref="E110:F110"/>
-    <mergeCell ref="C111:D111"/>
-    <mergeCell ref="E111:F111"/>
-    <mergeCell ref="C106:D106"/>
-    <mergeCell ref="E106:F106"/>
-    <mergeCell ref="C107:D107"/>
-    <mergeCell ref="E107:F107"/>
-    <mergeCell ref="C108:D108"/>
-    <mergeCell ref="E108:F108"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="C121:D121"/>
-    <mergeCell ref="E121:F121"/>
-    <mergeCell ref="C118:D118"/>
-    <mergeCell ref="E118:F118"/>
-    <mergeCell ref="C119:D119"/>
-    <mergeCell ref="E119:F119"/>
-    <mergeCell ref="C120:D120"/>
-    <mergeCell ref="E120:F120"/>
-    <mergeCell ref="C115:D115"/>
-    <mergeCell ref="E115:F115"/>
-    <mergeCell ref="C116:D116"/>
-    <mergeCell ref="E116:F116"/>
-    <mergeCell ref="C117:D117"/>
-    <mergeCell ref="E117:F117"/>
-    <mergeCell ref="C112:D112"/>
-    <mergeCell ref="E112:F112"/>
-    <mergeCell ref="C113:D113"/>
-    <mergeCell ref="E113:F113"/>
-    <mergeCell ref="C114:D114"/>
-    <mergeCell ref="E114:F114"/>
-    <mergeCell ref="C109:D109"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
normally fix for land assignement for each farm, need to restart for testing (vscode down)
</commit_message>
<xml_diff>
--- a/src/main/data/statistical_data/canton_stats.xlsx
+++ b/src/main/data/statistical_data/canton_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/douglasbouchet/Desktop/SwissFarmSimulation/src/main/data/statistical_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD2FB28C-30AF-354C-9F50-47AF474BC8CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACDE6E8-B974-4746-A821-36AC0212A7C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="500" windowWidth="17280" windowHeight="15640" xr2:uid="{98662E0A-59F8-1C4D-93E1-B3BF32019C75}"/>
   </bookViews>
@@ -645,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A78F01E-8977-B047-9AC9-A572E69C8992}">
   <dimension ref="A1:T122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="75" zoomScaleNormal="44" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+    <sheetView tabSelected="1" topLeftCell="J2" zoomScale="75" zoomScaleNormal="44" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
puting methods inside class Generator
</commit_message>
<xml_diff>
--- a/src/main/data/statistical_data/canton_stats.xlsx
+++ b/src/main/data/statistical_data/canton_stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/douglasbouchet/Desktop/SwissFarmSimulation/src/main/data/statistical_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DACDE6E8-B974-4746-A821-36AC0212A7C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4101C8AB-37FB-9542-BD8B-CA6C62C7D2CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="500" windowWidth="17280" windowHeight="15640" xr2:uid="{98662E0A-59F8-1C4D-93E1-B3BF32019C75}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{98662E0A-59F8-1C4D-93E1-B3BF32019C75}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
   <si>
     <t>Suisse</t>
   </si>
@@ -196,15 +196,19 @@
   </si>
   <si>
     <t>surface (km^2)</t>
+  </si>
+  <si>
+    <t>population</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="###\ ###\ ##0"/>
+    <numFmt numFmtId="166" formatCode="#,###,##0__;\-#,###,##0__;0__;@__\ "/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -273,7 +277,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -310,22 +314,30 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -643,10 +655,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A78F01E-8977-B047-9AC9-A572E69C8992}">
-  <dimension ref="A1:T122"/>
+  <dimension ref="A1:Y122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J2" zoomScale="75" zoomScaleNormal="44" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="80" zoomScaleNormal="44" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -664,7 +676,7 @@
     <col min="15" max="15" width="15.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>27</v>
       </c>
@@ -710,8 +722,11 @@
       <c r="O1" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="P1" s="26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -757,15 +772,19 @@
       <c r="O2" s="20">
         <v>41284</v>
       </c>
-      <c r="P2" s="32" t="s">
+      <c r="P2" s="38">
+        <v>8606033</v>
+      </c>
+      <c r="Q2" s="26"/>
+      <c r="U2" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="V2" s="29"/>
+      <c r="W2" s="29"/>
+      <c r="X2" s="29"/>
+      <c r="Y2" s="29"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -811,11 +830,15 @@
       <c r="O3" s="23">
         <v>1729</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3" s="37">
+        <v>1539275</v>
+      </c>
+      <c r="Q3" s="25"/>
+      <c r="U3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -861,8 +884,12 @@
       <c r="O4" s="23">
         <v>5959</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="P4" s="37">
+        <v>1039474</v>
+      </c>
+      <c r="Q4" s="25"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -908,8 +935,12 @@
       <c r="O5" s="23">
         <v>1493</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="P5" s="37">
+        <v>413120</v>
+      </c>
+      <c r="Q5" s="25"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -955,8 +986,12 @@
       <c r="O6" s="23">
         <v>1076</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="P6" s="37">
+        <v>36703</v>
+      </c>
+      <c r="Q6" s="25"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1002,8 +1037,12 @@
       <c r="O7" s="23">
         <v>906</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="P7" s="37">
+        <v>160480</v>
+      </c>
+      <c r="Q7" s="25"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1049,8 +1088,12 @@
       <c r="O8" s="23">
         <v>490</v>
       </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="P8" s="37">
+        <v>37930</v>
+      </c>
+      <c r="Q8" s="25"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1096,8 +1139,12 @@
       <c r="O9" s="23">
         <v>275</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="P9" s="37">
+        <v>43087</v>
+      </c>
+      <c r="Q9" s="25"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1143,8 +1190,12 @@
       <c r="O10" s="23">
         <v>685</v>
       </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="P10" s="37">
+        <v>40590</v>
+      </c>
+      <c r="Q10" s="25"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1190,8 +1241,12 @@
       <c r="O11" s="23">
         <v>238</v>
       </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="P11" s="37">
+        <v>127642</v>
+      </c>
+      <c r="Q11" s="25"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1237,8 +1292,12 @@
       <c r="O12" s="23">
         <v>1670</v>
       </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="P12" s="37">
+        <v>321783</v>
+      </c>
+      <c r="Q12" s="25"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -1284,8 +1343,12 @@
       <c r="O13" s="23">
         <v>790</v>
       </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="P13" s="37">
+        <v>275247</v>
+      </c>
+      <c r="Q13" s="25"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>52</v>
       </c>
@@ -1331,8 +1394,12 @@
       <c r="O14" s="23">
         <v>37</v>
       </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="P14" s="37">
+        <v>195844</v>
+      </c>
+      <c r="Q14" s="25"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>51</v>
       </c>
@@ -1378,8 +1445,12 @@
       <c r="O15" s="23">
         <v>517</v>
       </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="P15" s="37">
+        <v>289468</v>
+      </c>
+      <c r="Q15" s="25"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1425,8 +1496,12 @@
       <c r="O16" s="23">
         <v>298</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P16" s="37">
+        <v>82348</v>
+      </c>
+      <c r="Q16" s="25"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -1472,8 +1547,12 @@
       <c r="O17" s="23">
         <v>242</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P17" s="37">
+        <v>55445</v>
+      </c>
+      <c r="Q17" s="25"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -1519,8 +1598,12 @@
       <c r="O18" s="23">
         <v>172</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P18" s="37">
+        <v>16128</v>
+      </c>
+      <c r="Q18" s="25"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -1566,8 +1649,12 @@
       <c r="O19" s="23">
         <v>2025</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P19" s="37">
+        <v>510734</v>
+      </c>
+      <c r="Q19" s="25"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -1613,8 +1700,12 @@
       <c r="O20" s="23">
         <v>7105</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P20" s="37">
+        <v>199021</v>
+      </c>
+      <c r="Q20" s="25"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
@@ -1660,8 +1751,12 @@
       <c r="O21" s="23">
         <v>1403</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P21" s="37">
+        <v>685845</v>
+      </c>
+      <c r="Q21" s="25"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -1707,8 +1802,12 @@
       <c r="O22" s="23">
         <v>991</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P22" s="37">
+        <v>279547</v>
+      </c>
+      <c r="Q22" s="25"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
@@ -1754,8 +1853,12 @@
       <c r="O23" s="23">
         <v>2812</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P23" s="37">
+        <v>351491</v>
+      </c>
+      <c r="Q23" s="25"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -1801,8 +1904,12 @@
       <c r="O24" s="23">
         <v>3212</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P24" s="37">
+        <v>805098</v>
+      </c>
+      <c r="Q24" s="25"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
@@ -1848,8 +1955,12 @@
       <c r="O25" s="23">
         <v>5224</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P25" s="37">
+        <v>345525</v>
+      </c>
+      <c r="Q25" s="25"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>50</v>
       </c>
@@ -1895,8 +2006,12 @@
       <c r="O26" s="23">
         <v>802</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P26" s="37">
+        <v>176496</v>
+      </c>
+      <c r="Q26" s="25"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>49</v>
       </c>
@@ -1942,8 +2057,12 @@
       <c r="O27" s="23">
         <v>282</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P27" s="37">
+        <v>504128</v>
+      </c>
+      <c r="Q27" s="25"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
@@ -1989,8 +2108,12 @@
       <c r="O28" s="23">
         <v>835</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P28" s="37">
+        <v>73584</v>
+      </c>
+      <c r="Q28" s="25"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1998,21 +2121,21 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:15" ht="31" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="25" t="s">
+      <c r="C30" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="D30" s="25"/>
-      <c r="E30" s="34" t="s">
+      <c r="D30" s="36"/>
+      <c r="E30" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="F30" s="34"/>
+      <c r="F30" s="31"/>
       <c r="G30" s="2" t="s">
         <v>36</v>
       </c>
@@ -2020,21 +2143,21 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B31" s="7">
         <v>4956978.3459999999</v>
       </c>
-      <c r="C31" s="29">
+      <c r="C31" s="32">
         <v>4743.6284385153003</v>
       </c>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29">
+      <c r="D31" s="32"/>
+      <c r="E31" s="32">
         <v>786006</v>
       </c>
-      <c r="F31" s="29"/>
+      <c r="F31" s="32"/>
       <c r="G31" s="7">
         <v>1213333.6240000001</v>
       </c>
@@ -2044,21 +2167,21 @@
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B32" s="4">
         <v>367535.78282135999</v>
       </c>
-      <c r="C32" s="26">
+      <c r="C32" s="30">
         <v>5032.4135682755004</v>
       </c>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26">
+      <c r="D32" s="30"/>
+      <c r="E32" s="30">
         <v>84607.123103959006</v>
       </c>
-      <c r="F32" s="26"/>
+      <c r="F32" s="30"/>
       <c r="G32" s="4">
         <v>79546.385950830998</v>
       </c>
@@ -2073,14 +2196,14 @@
       <c r="B33" s="4">
         <v>790573.43857691996</v>
       </c>
-      <c r="C33" s="26">
+      <c r="C33" s="30">
         <v>4120.1966179320998</v>
       </c>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26">
+      <c r="D33" s="30"/>
+      <c r="E33" s="30">
         <v>160691.23349658001</v>
       </c>
-      <c r="F33" s="26"/>
+      <c r="F33" s="30"/>
       <c r="G33" s="4">
         <v>234277.36790541999</v>
       </c>
@@ -2095,14 +2218,14 @@
       <c r="B34" s="4">
         <v>483491.85653694998</v>
       </c>
-      <c r="C34" s="26">
+      <c r="C34" s="30">
         <v>6384.9391675662</v>
       </c>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26">
+      <c r="D34" s="30"/>
+      <c r="E34" s="30">
         <v>28920.746815546001</v>
       </c>
-      <c r="F34" s="26"/>
+      <c r="F34" s="30"/>
       <c r="G34" s="4">
         <v>106871.96583112</v>
       </c>
@@ -2117,14 +2240,14 @@
       <c r="B35" s="4">
         <v>13127.880841038001</v>
       </c>
-      <c r="C35" s="26">
+      <c r="C35" s="30">
         <v>1943.9784456084001</v>
       </c>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26">
+      <c r="D35" s="30"/>
+      <c r="E35" s="30">
         <v>5.1154354263000004</v>
       </c>
-      <c r="F35" s="26"/>
+      <c r="F35" s="30"/>
       <c r="G35" s="4">
         <v>8425.2740806111997</v>
       </c>
@@ -2139,14 +2262,14 @@
       <c r="B36" s="4">
         <v>58019.01410606</v>
       </c>
-      <c r="C36" s="26">
+      <c r="C36" s="30">
         <v>2452.3331419757001</v>
       </c>
-      <c r="D36" s="26"/>
-      <c r="E36" s="26">
+      <c r="D36" s="30"/>
+      <c r="E36" s="30">
         <v>339.49531817550002</v>
       </c>
-      <c r="F36" s="26"/>
+      <c r="F36" s="30"/>
       <c r="G36" s="4">
         <v>29891.684353421999</v>
       </c>
@@ -2161,14 +2284,14 @@
       <c r="B37" s="4">
         <v>34961.992935404996</v>
       </c>
-      <c r="C37" s="26">
+      <c r="C37" s="30">
         <v>4484.2614646646998</v>
       </c>
-      <c r="D37" s="26"/>
-      <c r="E37" s="26">
+      <c r="D37" s="30"/>
+      <c r="E37" s="30">
         <v>1.4441788682000001</v>
       </c>
-      <c r="F37" s="26"/>
+      <c r="F37" s="30"/>
       <c r="G37" s="4">
         <v>10736.300903747</v>
       </c>
@@ -2183,14 +2306,14 @@
       <c r="B38" s="4">
         <v>17345.379437226002</v>
       </c>
-      <c r="C38" s="26">
+      <c r="C38" s="30">
         <v>2926.6011063687001</v>
       </c>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26">
+      <c r="D38" s="30"/>
+      <c r="E38" s="30">
         <v>18.052235852399999</v>
       </c>
-      <c r="F38" s="26"/>
+      <c r="F38" s="30"/>
       <c r="G38" s="4">
         <v>7745.6980859078003</v>
       </c>
@@ -2205,14 +2328,14 @@
       <c r="B39" s="4">
         <v>22457.544221669999</v>
       </c>
-      <c r="C39" s="26">
+      <c r="C39" s="30">
         <v>3222.1217569615001</v>
       </c>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26">
+      <c r="D39" s="30"/>
+      <c r="E39" s="30">
         <v>64.043111324600005</v>
       </c>
-      <c r="F39" s="26"/>
+      <c r="F39" s="30"/>
       <c r="G39" s="4">
         <v>11</v>
       </c>
@@ -2227,14 +2350,14 @@
       <c r="B40" s="4">
         <v>45780.790559838002</v>
       </c>
-      <c r="C40" s="26">
+      <c r="C40" s="30">
         <v>4298.3429000486003</v>
       </c>
-      <c r="D40" s="26"/>
-      <c r="E40" s="26">
+      <c r="D40" s="30"/>
+      <c r="E40" s="30">
         <v>2535.3539956496002</v>
       </c>
-      <c r="F40" s="26"/>
+      <c r="F40" s="30"/>
       <c r="G40" s="4">
         <v>14660.921634013999</v>
       </c>
@@ -2249,14 +2372,14 @@
       <c r="B41" s="4">
         <v>339106.44353564002</v>
       </c>
-      <c r="C41" s="26">
+      <c r="C41" s="30">
         <v>4519.4547907927999</v>
       </c>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26">
+      <c r="D41" s="30"/>
+      <c r="E41" s="30">
         <v>69599.448877222007</v>
       </c>
-      <c r="F41" s="26"/>
+      <c r="F41" s="30"/>
       <c r="G41" s="4">
         <v>94235.858109088003</v>
       </c>
@@ -2271,14 +2394,14 @@
       <c r="B42" s="4">
         <v>75225.255770980002</v>
       </c>
-      <c r="C42" s="26">
+      <c r="C42" s="30">
         <v>2389.6053954861</v>
       </c>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26">
+      <c r="D42" s="30"/>
+      <c r="E42" s="30">
         <v>26893.706113788001</v>
       </c>
-      <c r="F42" s="26"/>
+      <c r="F42" s="30"/>
       <c r="G42" s="4">
         <v>36449.714810334997</v>
       </c>
@@ -2293,14 +2416,14 @@
       <c r="B43" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C43" s="27" t="s">
+      <c r="C43" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="D43" s="27"/>
-      <c r="E43" s="27" t="s">
+      <c r="D43" s="35"/>
+      <c r="E43" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="F43" s="27"/>
+      <c r="F43" s="35"/>
       <c r="G43" s="10" t="s">
         <v>31</v>
       </c>
@@ -2315,14 +2438,14 @@
       <c r="B44" s="4">
         <v>71845.928613395998</v>
       </c>
-      <c r="C44" s="26">
+      <c r="C44" s="30">
         <v>3286.5487961628</v>
       </c>
-      <c r="D44" s="26"/>
-      <c r="E44" s="26">
+      <c r="D44" s="30"/>
+      <c r="E44" s="30">
         <v>12636.640261428</v>
       </c>
-      <c r="F44" s="26"/>
+      <c r="F44" s="30"/>
       <c r="G44" s="4">
         <v>26220.550055222</v>
       </c>
@@ -2337,14 +2460,14 @@
       <c r="B45" s="4">
         <v>69521.910218307996</v>
       </c>
-      <c r="C45" s="26">
+      <c r="C45" s="30">
         <v>4402.4056927208003</v>
       </c>
-      <c r="D45" s="26"/>
-      <c r="E45" s="26">
+      <c r="D45" s="30"/>
+      <c r="E45" s="30">
         <v>30931.552146278002</v>
       </c>
-      <c r="F45" s="26"/>
+      <c r="F45" s="30"/>
       <c r="G45" s="4">
         <v>13455.576233948001</v>
       </c>
@@ -2359,14 +2482,14 @@
       <c r="B46" s="4">
         <v>34286.684238684</v>
       </c>
-      <c r="C46" s="26">
+      <c r="C46" s="30">
         <v>2892.2439402670998</v>
       </c>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26">
+      <c r="D46" s="30"/>
+      <c r="E46" s="30">
         <v>7.4430031184000001</v>
       </c>
-      <c r="F46" s="26"/>
+      <c r="F46" s="30"/>
       <c r="G46" s="4">
         <v>15791.405146641</v>
       </c>
@@ -2381,14 +2504,14 @@
       <c r="B47" s="4">
         <v>26062.397327483999</v>
       </c>
-      <c r="C47" s="26">
+      <c r="C47" s="30">
         <v>3647.4371382265999</v>
       </c>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26">
+      <c r="D47" s="30"/>
+      <c r="E47" s="30">
         <v>30.932318284200001</v>
       </c>
-      <c r="F47" s="26"/>
+      <c r="F47" s="30"/>
       <c r="G47" s="4">
         <v>9098.7580289252001</v>
       </c>
@@ -2403,14 +2526,14 @@
       <c r="B48" s="4">
         <v>306636.23944643</v>
       </c>
-      <c r="C48" s="26">
+      <c r="C48" s="30">
         <v>4294.4146918068</v>
       </c>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26">
+      <c r="D48" s="30"/>
+      <c r="E48" s="30">
         <v>10312.198204822</v>
       </c>
-      <c r="F48" s="26"/>
+      <c r="F48" s="30"/>
       <c r="G48" s="4">
         <v>97031.900358654995</v>
       </c>
@@ -2425,14 +2548,14 @@
       <c r="B49" s="4">
         <v>168043.5919497</v>
       </c>
-      <c r="C49" s="26">
+      <c r="C49" s="30">
         <v>2999.0807337578999</v>
       </c>
-      <c r="D49" s="26"/>
-      <c r="E49" s="26">
+      <c r="D49" s="30"/>
+      <c r="E49" s="30">
         <v>4578.4777773425003</v>
       </c>
-      <c r="F49" s="26"/>
+      <c r="F49" s="30"/>
       <c r="G49" s="4">
         <v>60260.898596421997</v>
       </c>
@@ -2447,14 +2570,14 @@
       <c r="B50" s="4">
         <v>315691.20352842001</v>
       </c>
-      <c r="C50" s="26">
+      <c r="C50" s="30">
         <v>5261.7129882831996</v>
       </c>
-      <c r="D50" s="26"/>
-      <c r="E50" s="26">
+      <c r="D50" s="30"/>
+      <c r="E50" s="30">
         <v>67337.303038038997</v>
       </c>
-      <c r="F50" s="26"/>
+      <c r="F50" s="30"/>
       <c r="G50" s="4">
         <v>68500.514683921007</v>
       </c>
@@ -2469,14 +2592,14 @@
       <c r="B51" s="4">
         <v>404753.06168148998</v>
       </c>
-      <c r="C51" s="26">
+      <c r="C51" s="30">
         <v>8184.1208365734001</v>
       </c>
-      <c r="D51" s="26"/>
-      <c r="E51" s="26">
+      <c r="D51" s="30"/>
+      <c r="E51" s="30">
         <v>54666.647685978001</v>
       </c>
-      <c r="F51" s="26"/>
+      <c r="F51" s="30"/>
       <c r="G51" s="4">
         <v>59512.903082156001</v>
       </c>
@@ -2491,14 +2614,14 @@
       <c r="B52" s="4">
         <v>60062.907964227001</v>
       </c>
-      <c r="C52" s="26">
+      <c r="C52" s="30">
         <v>4377.9863378034997</v>
       </c>
-      <c r="D52" s="26"/>
-      <c r="E52" s="26">
+      <c r="D52" s="30"/>
+      <c r="E52" s="30">
         <v>3063.3489903262998</v>
       </c>
-      <c r="F52" s="26"/>
+      <c r="F52" s="30"/>
       <c r="G52" s="4">
         <v>13190.965869324</v>
       </c>
@@ -2513,14 +2636,14 @@
       <c r="B53" s="4">
         <v>585987.36389144999</v>
       </c>
-      <c r="C53" s="26">
+      <c r="C53" s="30">
         <v>5393.0412060375002</v>
       </c>
-      <c r="D53" s="26"/>
-      <c r="E53" s="26">
+      <c r="D53" s="30"/>
+      <c r="E53" s="30">
         <v>172588.86868720001</v>
       </c>
-      <c r="F53" s="26"/>
+      <c r="F53" s="30"/>
       <c r="G53" s="4">
         <v>96180.677173251999</v>
       </c>
@@ -2535,14 +2658,14 @@
       <c r="B54" s="4">
         <v>323692.26819764002</v>
       </c>
-      <c r="C54" s="26">
+      <c r="C54" s="30">
         <v>8779.2620089894008</v>
       </c>
-      <c r="D54" s="26"/>
-      <c r="E54" s="26">
+      <c r="D54" s="30"/>
+      <c r="E54" s="30">
         <v>5990.4473537923004</v>
       </c>
-      <c r="F54" s="26"/>
+      <c r="F54" s="30"/>
       <c r="G54" s="4">
         <v>30877.321384491999</v>
       </c>
@@ -2557,14 +2680,14 @@
       <c r="B55" s="4">
         <v>119009.67327607999</v>
       </c>
-      <c r="C55" s="26">
+      <c r="C55" s="30">
         <v>3775.0408647021</v>
       </c>
-      <c r="D55" s="26"/>
-      <c r="E55" s="26">
+      <c r="D55" s="30"/>
+      <c r="E55" s="30">
         <v>9868.4417303231003</v>
       </c>
-      <c r="F55" s="26"/>
+      <c r="F55" s="30"/>
       <c r="G55" s="4">
         <v>36372.944998935003</v>
       </c>
@@ -2579,14 +2702,14 @@
       <c r="B56" s="4">
         <v>118085.59849824</v>
       </c>
-      <c r="C56" s="26">
+      <c r="C56" s="30">
         <v>10437.398773012999</v>
       </c>
-      <c r="D56" s="26"/>
-      <c r="E56" s="26">
+      <c r="D56" s="30"/>
+      <c r="E56" s="30">
         <v>17055.58471521</v>
       </c>
-      <c r="F56" s="26"/>
+      <c r="F56" s="30"/>
       <c r="G56" s="4">
         <v>5912.5978597676003</v>
       </c>
@@ -2601,14 +2724,14 @@
       <c r="B57" s="4">
         <v>105674.13735413</v>
       </c>
-      <c r="C57" s="26">
+      <c r="C57" s="30">
         <v>2612.7022089568</v>
       </c>
-      <c r="D57" s="26"/>
-      <c r="E57" s="26">
+      <c r="D57" s="30"/>
+      <c r="E57" s="30">
         <v>23262.760456905002</v>
       </c>
-      <c r="F57" s="26"/>
+      <c r="F57" s="30"/>
       <c r="G57" s="4">
         <v>49012.977698084003</v>
       </c>
@@ -3064,10 +3187,10 @@
     <row r="94" spans="1:13" ht="31" x14ac:dyDescent="0.35">
       <c r="A94" s="11"/>
       <c r="B94" s="3"/>
-      <c r="C94" s="30"/>
-      <c r="D94" s="30"/>
-      <c r="E94" s="31"/>
-      <c r="F94" s="31"/>
+      <c r="C94" s="33"/>
+      <c r="D94" s="33"/>
+      <c r="E94" s="34"/>
+      <c r="F94" s="34"/>
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
       <c r="I94" s="1"/>
@@ -3079,10 +3202,10 @@
     <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95" s="3"/>
       <c r="B95" s="8"/>
-      <c r="C95" s="28"/>
-      <c r="D95" s="28"/>
-      <c r="E95" s="28"/>
-      <c r="F95" s="28"/>
+      <c r="C95" s="27"/>
+      <c r="D95" s="27"/>
+      <c r="E95" s="27"/>
+      <c r="F95" s="27"/>
       <c r="G95" s="8"/>
       <c r="H95" s="8"/>
       <c r="I95" s="1"/>
@@ -3094,10 +3217,10 @@
     <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96" s="3"/>
       <c r="B96" s="8"/>
-      <c r="C96" s="28"/>
-      <c r="D96" s="28"/>
-      <c r="E96" s="28"/>
-      <c r="F96" s="28"/>
+      <c r="C96" s="27"/>
+      <c r="D96" s="27"/>
+      <c r="E96" s="27"/>
+      <c r="F96" s="27"/>
       <c r="G96" s="8"/>
       <c r="H96" s="8"/>
       <c r="I96" s="1"/>
@@ -3109,10 +3232,10 @@
     <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97" s="3"/>
       <c r="B97" s="8"/>
-      <c r="C97" s="28"/>
-      <c r="D97" s="28"/>
-      <c r="E97" s="28"/>
-      <c r="F97" s="28"/>
+      <c r="C97" s="27"/>
+      <c r="D97" s="27"/>
+      <c r="E97" s="27"/>
+      <c r="F97" s="27"/>
       <c r="G97" s="8"/>
       <c r="H97" s="8"/>
       <c r="I97" s="1"/>
@@ -3124,10 +3247,10 @@
     <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98" s="3"/>
       <c r="B98" s="8"/>
-      <c r="C98" s="28"/>
-      <c r="D98" s="28"/>
-      <c r="E98" s="28"/>
-      <c r="F98" s="28"/>
+      <c r="C98" s="27"/>
+      <c r="D98" s="27"/>
+      <c r="E98" s="27"/>
+      <c r="F98" s="27"/>
       <c r="G98" s="8"/>
       <c r="H98" s="8"/>
       <c r="I98" s="1"/>
@@ -3139,10 +3262,10 @@
     <row r="99" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A99" s="3"/>
       <c r="B99" s="8"/>
-      <c r="C99" s="28"/>
-      <c r="D99" s="28"/>
-      <c r="E99" s="28"/>
-      <c r="F99" s="28"/>
+      <c r="C99" s="27"/>
+      <c r="D99" s="27"/>
+      <c r="E99" s="27"/>
+      <c r="F99" s="27"/>
       <c r="G99" s="8"/>
       <c r="H99" s="8"/>
       <c r="I99" s="1"/>
@@ -3154,10 +3277,10 @@
     <row r="100" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A100" s="3"/>
       <c r="B100" s="8"/>
-      <c r="C100" s="28"/>
-      <c r="D100" s="28"/>
-      <c r="E100" s="28"/>
-      <c r="F100" s="28"/>
+      <c r="C100" s="27"/>
+      <c r="D100" s="27"/>
+      <c r="E100" s="27"/>
+      <c r="F100" s="27"/>
       <c r="G100" s="8"/>
       <c r="H100" s="8"/>
       <c r="I100" s="1"/>
@@ -3169,10 +3292,10 @@
     <row r="101" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A101" s="3"/>
       <c r="B101" s="8"/>
-      <c r="C101" s="28"/>
-      <c r="D101" s="28"/>
-      <c r="E101" s="28"/>
-      <c r="F101" s="28"/>
+      <c r="C101" s="27"/>
+      <c r="D101" s="27"/>
+      <c r="E101" s="27"/>
+      <c r="F101" s="27"/>
       <c r="G101" s="8"/>
       <c r="H101" s="8"/>
       <c r="I101" s="1"/>
@@ -3184,10 +3307,10 @@
     <row r="102" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A102" s="3"/>
       <c r="B102" s="8"/>
-      <c r="C102" s="28"/>
-      <c r="D102" s="28"/>
-      <c r="E102" s="28"/>
-      <c r="F102" s="28"/>
+      <c r="C102" s="27"/>
+      <c r="D102" s="27"/>
+      <c r="E102" s="27"/>
+      <c r="F102" s="27"/>
       <c r="G102" s="8"/>
       <c r="H102" s="8"/>
       <c r="I102" s="1"/>
@@ -3199,10 +3322,10 @@
     <row r="103" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A103" s="3"/>
       <c r="B103" s="8"/>
-      <c r="C103" s="28"/>
-      <c r="D103" s="28"/>
-      <c r="E103" s="28"/>
-      <c r="F103" s="28"/>
+      <c r="C103" s="27"/>
+      <c r="D103" s="27"/>
+      <c r="E103" s="27"/>
+      <c r="F103" s="27"/>
       <c r="G103" s="8"/>
       <c r="H103" s="8"/>
       <c r="I103" s="1"/>
@@ -3214,10 +3337,10 @@
     <row r="104" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A104" s="3"/>
       <c r="B104" s="8"/>
-      <c r="C104" s="28"/>
-      <c r="D104" s="28"/>
-      <c r="E104" s="28"/>
-      <c r="F104" s="28"/>
+      <c r="C104" s="27"/>
+      <c r="D104" s="27"/>
+      <c r="E104" s="27"/>
+      <c r="F104" s="27"/>
       <c r="G104" s="8"/>
       <c r="H104" s="8"/>
       <c r="I104" s="1"/>
@@ -3229,10 +3352,10 @@
     <row r="105" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A105" s="3"/>
       <c r="B105" s="8"/>
-      <c r="C105" s="28"/>
-      <c r="D105" s="28"/>
-      <c r="E105" s="28"/>
-      <c r="F105" s="28"/>
+      <c r="C105" s="27"/>
+      <c r="D105" s="27"/>
+      <c r="E105" s="27"/>
+      <c r="F105" s="27"/>
       <c r="G105" s="8"/>
       <c r="H105" s="8"/>
       <c r="I105" s="1"/>
@@ -3244,10 +3367,10 @@
     <row r="106" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A106" s="3"/>
       <c r="B106" s="8"/>
-      <c r="C106" s="28"/>
-      <c r="D106" s="28"/>
-      <c r="E106" s="28"/>
-      <c r="F106" s="28"/>
+      <c r="C106" s="27"/>
+      <c r="D106" s="27"/>
+      <c r="E106" s="27"/>
+      <c r="F106" s="27"/>
       <c r="G106" s="8"/>
       <c r="H106" s="8"/>
       <c r="I106" s="1"/>
@@ -3259,10 +3382,10 @@
     <row r="107" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A107" s="3"/>
       <c r="B107" s="13"/>
-      <c r="C107" s="33"/>
-      <c r="D107" s="33"/>
-      <c r="E107" s="33"/>
-      <c r="F107" s="33"/>
+      <c r="C107" s="28"/>
+      <c r="D107" s="28"/>
+      <c r="E107" s="28"/>
+      <c r="F107" s="28"/>
       <c r="G107" s="13"/>
       <c r="H107" s="13"/>
       <c r="I107" s="1"/>
@@ -3274,10 +3397,10 @@
     <row r="108" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A108" s="3"/>
       <c r="B108" s="8"/>
-      <c r="C108" s="28"/>
-      <c r="D108" s="28"/>
-      <c r="E108" s="28"/>
-      <c r="F108" s="28"/>
+      <c r="C108" s="27"/>
+      <c r="D108" s="27"/>
+      <c r="E108" s="27"/>
+      <c r="F108" s="27"/>
       <c r="G108" s="8"/>
       <c r="H108" s="8"/>
       <c r="I108" s="1"/>
@@ -3289,10 +3412,10 @@
     <row r="109" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A109" s="3"/>
       <c r="B109" s="8"/>
-      <c r="C109" s="28"/>
-      <c r="D109" s="28"/>
-      <c r="E109" s="28"/>
-      <c r="F109" s="28"/>
+      <c r="C109" s="27"/>
+      <c r="D109" s="27"/>
+      <c r="E109" s="27"/>
+      <c r="F109" s="27"/>
       <c r="G109" s="8"/>
       <c r="H109" s="8"/>
       <c r="I109" s="1"/>
@@ -3304,10 +3427,10 @@
     <row r="110" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A110" s="3"/>
       <c r="B110" s="8"/>
-      <c r="C110" s="28"/>
-      <c r="D110" s="28"/>
-      <c r="E110" s="28"/>
-      <c r="F110" s="28"/>
+      <c r="C110" s="27"/>
+      <c r="D110" s="27"/>
+      <c r="E110" s="27"/>
+      <c r="F110" s="27"/>
       <c r="G110" s="8"/>
       <c r="H110" s="8"/>
       <c r="I110" s="1"/>
@@ -3319,10 +3442,10 @@
     <row r="111" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A111" s="3"/>
       <c r="B111" s="8"/>
-      <c r="C111" s="28"/>
-      <c r="D111" s="28"/>
-      <c r="E111" s="28"/>
-      <c r="F111" s="28"/>
+      <c r="C111" s="27"/>
+      <c r="D111" s="27"/>
+      <c r="E111" s="27"/>
+      <c r="F111" s="27"/>
       <c r="G111" s="8"/>
       <c r="H111" s="8"/>
       <c r="I111" s="1"/>
@@ -3334,10 +3457,10 @@
     <row r="112" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A112" s="3"/>
       <c r="B112" s="8"/>
-      <c r="C112" s="28"/>
-      <c r="D112" s="28"/>
-      <c r="E112" s="28"/>
-      <c r="F112" s="28"/>
+      <c r="C112" s="27"/>
+      <c r="D112" s="27"/>
+      <c r="E112" s="27"/>
+      <c r="F112" s="27"/>
       <c r="G112" s="8"/>
       <c r="H112" s="8"/>
       <c r="I112" s="1"/>
@@ -3349,10 +3472,10 @@
     <row r="113" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A113" s="3"/>
       <c r="B113" s="8"/>
-      <c r="C113" s="28"/>
-      <c r="D113" s="28"/>
-      <c r="E113" s="28"/>
-      <c r="F113" s="28"/>
+      <c r="C113" s="27"/>
+      <c r="D113" s="27"/>
+      <c r="E113" s="27"/>
+      <c r="F113" s="27"/>
       <c r="G113" s="8"/>
       <c r="H113" s="8"/>
       <c r="I113" s="1"/>
@@ -3364,10 +3487,10 @@
     <row r="114" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A114" s="3"/>
       <c r="B114" s="8"/>
-      <c r="C114" s="28"/>
-      <c r="D114" s="28"/>
-      <c r="E114" s="28"/>
-      <c r="F114" s="28"/>
+      <c r="C114" s="27"/>
+      <c r="D114" s="27"/>
+      <c r="E114" s="27"/>
+      <c r="F114" s="27"/>
       <c r="G114" s="8"/>
       <c r="H114" s="8"/>
       <c r="I114" s="1"/>
@@ -3379,10 +3502,10 @@
     <row r="115" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A115" s="3"/>
       <c r="B115" s="8"/>
-      <c r="C115" s="28"/>
-      <c r="D115" s="28"/>
-      <c r="E115" s="28"/>
-      <c r="F115" s="28"/>
+      <c r="C115" s="27"/>
+      <c r="D115" s="27"/>
+      <c r="E115" s="27"/>
+      <c r="F115" s="27"/>
       <c r="G115" s="8"/>
       <c r="H115" s="8"/>
       <c r="I115" s="1"/>
@@ -3394,10 +3517,10 @@
     <row r="116" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A116" s="3"/>
       <c r="B116" s="8"/>
-      <c r="C116" s="28"/>
-      <c r="D116" s="28"/>
-      <c r="E116" s="28"/>
-      <c r="F116" s="28"/>
+      <c r="C116" s="27"/>
+      <c r="D116" s="27"/>
+      <c r="E116" s="27"/>
+      <c r="F116" s="27"/>
       <c r="G116" s="8"/>
       <c r="H116" s="8"/>
       <c r="I116" s="1"/>
@@ -3409,10 +3532,10 @@
     <row r="117" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A117" s="3"/>
       <c r="B117" s="8"/>
-      <c r="C117" s="28"/>
-      <c r="D117" s="28"/>
-      <c r="E117" s="28"/>
-      <c r="F117" s="28"/>
+      <c r="C117" s="27"/>
+      <c r="D117" s="27"/>
+      <c r="E117" s="27"/>
+      <c r="F117" s="27"/>
       <c r="G117" s="8"/>
       <c r="H117" s="8"/>
       <c r="I117" s="1"/>
@@ -3424,10 +3547,10 @@
     <row r="118" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A118" s="3"/>
       <c r="B118" s="8"/>
-      <c r="C118" s="28"/>
-      <c r="D118" s="28"/>
-      <c r="E118" s="28"/>
-      <c r="F118" s="28"/>
+      <c r="C118" s="27"/>
+      <c r="D118" s="27"/>
+      <c r="E118" s="27"/>
+      <c r="F118" s="27"/>
       <c r="G118" s="8"/>
       <c r="H118" s="8"/>
       <c r="I118" s="1"/>
@@ -3439,10 +3562,10 @@
     <row r="119" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A119" s="3"/>
       <c r="B119" s="8"/>
-      <c r="C119" s="28"/>
-      <c r="D119" s="28"/>
-      <c r="E119" s="28"/>
-      <c r="F119" s="28"/>
+      <c r="C119" s="27"/>
+      <c r="D119" s="27"/>
+      <c r="E119" s="27"/>
+      <c r="F119" s="27"/>
       <c r="G119" s="8"/>
       <c r="H119" s="8"/>
       <c r="I119" s="1"/>
@@ -3454,10 +3577,10 @@
     <row r="120" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A120" s="3"/>
       <c r="B120" s="8"/>
-      <c r="C120" s="28"/>
-      <c r="D120" s="28"/>
-      <c r="E120" s="28"/>
-      <c r="F120" s="28"/>
+      <c r="C120" s="27"/>
+      <c r="D120" s="27"/>
+      <c r="E120" s="27"/>
+      <c r="F120" s="27"/>
       <c r="G120" s="8"/>
       <c r="H120" s="8"/>
       <c r="I120" s="1"/>
@@ -3469,10 +3592,10 @@
     <row r="121" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A121" s="3"/>
       <c r="B121" s="8"/>
-      <c r="C121" s="28"/>
-      <c r="D121" s="28"/>
-      <c r="E121" s="28"/>
-      <c r="F121" s="28"/>
+      <c r="C121" s="27"/>
+      <c r="D121" s="27"/>
+      <c r="E121" s="27"/>
+      <c r="F121" s="27"/>
       <c r="G121" s="8"/>
       <c r="H121" s="8"/>
       <c r="I121" s="1"/>
@@ -3498,6 +3621,95 @@
     </row>
   </sheetData>
   <mergeCells count="113">
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="E97:F97"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="E98:F98"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="E99:F99"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="E94:F94"/>
+    <mergeCell ref="C95:D95"/>
+    <mergeCell ref="E95:F95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="E96:F96"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="C111:D111"/>
+    <mergeCell ref="E111:F111"/>
+    <mergeCell ref="C106:D106"/>
+    <mergeCell ref="E106:F106"/>
+    <mergeCell ref="C107:D107"/>
+    <mergeCell ref="E107:F107"/>
+    <mergeCell ref="C108:D108"/>
+    <mergeCell ref="E108:F108"/>
+    <mergeCell ref="U2:Y2"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="C103:D103"/>
+    <mergeCell ref="E103:F103"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="E104:F104"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="E105:F105"/>
+    <mergeCell ref="C100:D100"/>
+    <mergeCell ref="E100:F100"/>
+    <mergeCell ref="C101:D101"/>
+    <mergeCell ref="E101:F101"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="E102:F102"/>
     <mergeCell ref="C112:D112"/>
     <mergeCell ref="E112:F112"/>
     <mergeCell ref="C113:D113"/>
@@ -3522,95 +3734,6 @@
     <mergeCell ref="E109:F109"/>
     <mergeCell ref="C110:D110"/>
     <mergeCell ref="E110:F110"/>
-    <mergeCell ref="C111:D111"/>
-    <mergeCell ref="E111:F111"/>
-    <mergeCell ref="C106:D106"/>
-    <mergeCell ref="E106:F106"/>
-    <mergeCell ref="C107:D107"/>
-    <mergeCell ref="E107:F107"/>
-    <mergeCell ref="C108:D108"/>
-    <mergeCell ref="E108:F108"/>
-    <mergeCell ref="P2:T2"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="C103:D103"/>
-    <mergeCell ref="E103:F103"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="E104:F104"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="E105:F105"/>
-    <mergeCell ref="C100:D100"/>
-    <mergeCell ref="E100:F100"/>
-    <mergeCell ref="C101:D101"/>
-    <mergeCell ref="E101:F101"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="E102:F102"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="E97:F97"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="E98:F98"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="E99:F99"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="E94:F94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="E95:F95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="E96:F96"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="E51:F51"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>